<commit_message>
Get daily reddit data: Tue Sep 17 08:10:17 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_09_22.xlsx
+++ b/data/collected_data/2024_09_22.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C491"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,3236 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1fit8zv</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>Never done my nails before, apart from this whole chipping malarkey I think they came out nice</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qzfxp4xvrbpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1fit0uj</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>Pink New nails</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n0exafolpbpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1firb78</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>I mean I like my fall mani. But I love who these nails were trying to grab! Swipe to see...</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1firb78</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1firz0e</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>Vacation nails</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/75t0huvbdbpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1firh0n</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>Got my nails done</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1firh0n</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1firgar</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t xml:space="preserve">what is an acceptable amount of time between getting new acrylics? </t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1firgar/what_is_an_acceptable_amount_of_time_between/</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1firbx0</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1st attempt ever at doing nail extension, can you two which two nails? </t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s44y1ucb6bpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1fiqu15</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Saw this while scrolling… zoomed in to screenshot because what in the world </t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1pqc51kv0bpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1fiqkvw</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>New self-done mani 😁</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fiqkvw</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1fipvk0</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails I painted </t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fipvk0</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1fipuw8</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is there another nail polish with this color? The brand got discontinued and its one of my favs </t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g6qzhcf7rapd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1fipp9z</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>New Improved Impress Nails</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yd8fd3zppapd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1fiof7b</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What color would you choose for your next dip manicure? </t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fiof7b</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1fiifep</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>Edjy nail cutter</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fiifep/edjy_nail_cutter/</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1fiph9g</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>Is the Spider too much?</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fiph9g</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1fip9dn</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>Pumpkin vibes 🧡</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fip9dn</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1fip5hv</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>wedding nails.</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/joi9gyhlkapd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1fip3lc</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tips on how to get started </t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fip3lc/tips_on_how_to_get_started/</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1fiozu8</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>New set - building gel + gel polish</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gwg3m576japd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1fiocnk</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>Which colour nails for a wedding?</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fiocnk</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1fins58</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>After yeaaaars of trying I’ve finally managed a half decent almond shape on myself 🥹</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6sstr4wt8apd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1fil9n0</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>Question about spider gel</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fil9n0/question_about_spider_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1fidklt</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My friend got her nails done and I want something like it...what is this called?? </t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fidklt/my_friend_got_her_nails_done_and_i_want_something/</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1fifx78</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Therapeutic </t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zinaeydbk8pd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1fimxmz</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My nails I did </t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fimxmz</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1fimwms</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I did Beetle Juice nails 😁 </t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fimwms</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1fimr9e</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I got this new green today &amp; decided to do spooky season nails! yay or nay? </t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fimr9e</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1fildpt</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t xml:space="preserve">🤎 </t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qihqt8t2p9pd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1filbrb</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Obsessed! </t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q271maeoo9pd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1fil8wk</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I have tiny nail beds. Any brands of acrylics (preferably the predone ones, cuz I’m lazy) that may fit me decently? </t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yew37u02o9pd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1fil2a5</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>It’s fall people 🍂🍁🍃</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fil2a5</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1fijz47</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>A set for a friend</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fijz47</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1fijbta</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I started painting my own press ons! Here’s what I have so far. Any suggestions for future sets?? </t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fijbta</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1fii9q9</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>Simple designs, but these are my favorites so far 💅</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fii9q9</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1fii8xl</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How are these for the beginner? </t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/duehtbou09pd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1fii6hm</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is this a standard tipping policy? </t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k6dimfpb09pd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1fii1t3</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>Tis the season…</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x4w1xz7ez8pd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1fihip3</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>Love a colorful French tip 💖</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dmy9eqsiv8pd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1fih79m</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>New set of fall nails</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vfx1xp19t8pd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1figwv4</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>Got my nails done for the first time ever</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1figwv4</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1figrou</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fall nails ready! </t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lhog0a36q8pd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1figleu</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Autumnal attempt? </t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1figleu</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1fifwh3</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>can you change your design after gel?</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fifwh3/can_you_change_your_design_after_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1fifva5</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>Are essence press on nails good?</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/294x2e3yj8pd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1fiftay</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>Love love it</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7mjbi9yjj8pd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1fifafi</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New to nails but loving this new (half) set. Thinking of ditching the acrylic powder because I struggle so much with it. </t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zdcf13gvf8pd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1fifa31</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>Nearly finished my beetlejuice nail set! 🥳 Here is Bob! He's my fav 🥰💕 Hand painted on 10XL cover tips 🤩</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/81pf3k1tf8pd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1fiev2l</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>Casino themed acrylics!!</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fiev2l</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1fiesgk</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>I did this nail art today, what do you think?</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3e29mlocc8pd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1fier4w</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>The Autumnal Vibes have arrived 🍂</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sqxqp9b3c8pd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1fieo9x</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>Should I go back and ask to get this fixed?</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fieo9x</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1fiehbq</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>Spooky szn nails ❤️🩸</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fiehbq</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1fiecc4</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>por qué no los dos? 🤷‍♀️</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fiecc4</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1fie1xj</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>Fire</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fie1xj</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1fidtyg</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New nails for this week </t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aazjmkef58pd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1fid5cb</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>Pretty in pink 💕</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8a85ldni08pd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1fid2k9</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New day to practice something new on my press on nails </t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kbh3ah8yz7pd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1fichnv</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>Taking a break from gel while on maternity leave. Tips for making my natural nails look their best?</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fichnv/taking_a_break_from_gel_while_on_maternity_leave/</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1ficcoh</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>Stargirl ⭐💅🏾</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ficcoh</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1fic45x</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ready for fall 🌻 </t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xkd39eh4t7pd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1fic1j8</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>Any tips for applying nails?</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fic1j8/any_tips_for_applying_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1fiboyq</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>Hate how my nails look!</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a5dmd1g3q7pd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1fib9vu</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>✨️🌈Got my nails done🌈✨️</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lnjmd8w0n7pd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1fiaxgp</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>New Month, New Manicure</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fiaxgp</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1fiab4u</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love to create free style </t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/41s0ogpqf7pd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1fiaaim</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>How to replicate? This photo is from u/JDP623. It is a gel nail color with a matte top coat. But this specific dark grey/black color is everything I want in a polish. Help!</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c97iek0lf7pd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1fi9y90</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My first attempt at aura nails </t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0a93590hd7pd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1fi9y56</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>My nails during this year so far</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fi9y56</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1fi3z38</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gothic Romance inspired nails </t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fi3z38</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1fi7qmb</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Not exactly what I wanted but still soooo pretty!! </t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/28r32jn1y6pd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1fi9se2</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How long does a bottle of Gelcare gel polish last? </t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fi9se2/how_long_does_a_bottle_of_gelcare_gel_polish_last/</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1fi9qtz</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>My Wedding nails</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fi9qtz</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1fi9klv</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>🧡🤎</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9rp624hua7pd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1fi8z8a</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>Nail repair? Story in comments</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fi8z8a</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1fi8tmf</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>I love my pink nails🎀💗💅🏾</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q83qaeup57pd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1fi8gld</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>Skelly Hands 💀✨</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fi8gld</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1fi87ey</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>Dark red jelly nails with iridescent bow charms and flowers on a friend🩸🎀🥀</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fi87ey</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1fi84w0</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>I sculpted my first stiletto</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fi84w0</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1fi7wpy</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>Never have tried this color before, not sure how to feel 🫣</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/239vg798z6pd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1fi7bea</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>Autumn x 70s vibes</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eak4ervyu6pd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1fi758s</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>Help with sizing</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fi758s</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1fi6xrs</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Another attempt at press-on nails. ⚫️🦋💅🏼 </t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4bjy8388s6pd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1fi6p5e</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New set! </t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fi6p5e</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1fi6l63</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>I might just have to ask my nail tech for her hand in marriage lol</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fi6l63</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1fi65kt</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>chocolate glazed doughnut press-ons</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fi65kt</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1fi62s5</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My today’s nails 💅 </t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o1x14mdvl6pd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1fi627r</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>22 years old, first ever set!</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fi627r</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1fi5yn3</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>Free hand aquarium themed nails which glows in the dark.</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fi5yn3</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1fi5azc</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>my favorite set so far! 💕✨🎀</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8d2kb6x4g6pd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1fi57gc</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Foxy in Fall 🦊 </t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/27f5kszdf6pd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1fi51dh</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>No apex</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fi51dh</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1fi3xdz</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>Halloween nails</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v58jbthf56pd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1fi30bl</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>My hands don't look feminine so i often want my nails painted</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sq8hfzwjx5pd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1fi2zwt</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>What shape would suit my hands/nails?</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fi2zwt/what_shape_would_suit_my_handsnails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1fi2jk1</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>Broken nail🫡</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4dv0i3v9t5pd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1fi2fgp</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>I was doubting to have it in pink at first, but since my sister's birthday is coming in 3 days I have to make it her favorite color. I didn't expect it to look good on me 🩷🌸</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fi2fgp</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1fi04bk</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Yes o no ? I'm thinking of going to this pretty color </t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2xo9059n15pd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1fhzzf4</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>Made my friend and I some funky nailart 🤍</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rmo1b0tpz4pd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1fhzljz</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t xml:space="preserve">favourite set I’ve ever done </t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pt8b0ys5u4pd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1fisun3</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Baby laquerista </t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fisun3</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1fis0c4</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>What colors are these? (info in comments)</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ncco9mqqdbpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1firczy</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>end of summer themed mani ☀️💅🏼🌴</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3xuurzym6bpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1fircf0</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First attempt ever at nail extensions, can you tell which two nails? </t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0wxngmbg6bpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1fiqu6f</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>Iso recommendations: Super dark plum creme/crelly, almost black on the nail</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fiqu6f/iso_recommendations_super_dark_plum_cremecrelly/</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1fiok6f</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Need help fixing nail sidewalls! </t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fiok6f</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1fio7b4</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>ILNP- Shooting Star</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fio7b4</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1finhjh</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>to all the professional swatchers/brands out there</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1finhjh/to_all_the_professional_swatchersbrands_out_there/</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1fin7k3</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>Chanel Phenomene 189</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fin7k3</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1fim612</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>Clionadh Cosmetics Psilocybin magic ✨🍄</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/y7n07a4av9pd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1film9l</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>Accidentally twinning with my soda</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fgxgwunyq9pd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1fil3gx</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>A juicy pink for the last week of summer 💖</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sxqw0f3vm9pd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1fil12l</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t xml:space="preserve">“Cool Whip In My Hair” from LynB Designs’ Misheard Lyrics Collection. Please see comments where I mishear the rest of the song. </t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fil12l</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1fiktjd</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>The Psilocybin hype is real (plus 10lb vs 30lb vs ManiMag magnet test)</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fiktjd</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1fikcx6</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>goodbye summer 🍂</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s0bemd8vg9pd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1fik89n</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>Looking for luminous polishes</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fik89n/looking_for_luminous_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1fijzgl</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>Haunting Your Own House🤩dagnabbit EMILY DE MOLLYYYY</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fijzgl</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1fiitzb</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>Mani of the week: neutral :)</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fiitzb</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1fii2p2</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>lynb fall sale haul! 👻</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2wg8pdqkz8pd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1fii0ct</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>love the sparkling steely look</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fii0ct</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1fihsve</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>When you feel like skipping to spooky season with orange nails, but you also need to take professional product pictures that only show your thumb 😅</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t67smrl0x8pd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1fihpeg</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time getting extensions </t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fihpeg/first_time_getting_extensions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1fihazf</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Share your favorite purple shimmers! </t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0h7fotc0u8pd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1fih6vu</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>Dupe for Atomic Polish Sour Apple Rings?</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fih6vu</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1fih6l7</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>Dupe for Atomic Polish Sour Apple Rings?</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fih6l7</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1figwys</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>Love this darker green! 🌲</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1figwys</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1figv4y</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>🛸 if you wanna go and be stupid, don’t do it in front of me 🛸</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fzrlkzqqq8pd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1figotf</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>Black Opal Dupe?</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1figotf/black_opal_dupe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1figdgz</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Kitty manicure! </t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1figdgz</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1figakg</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Psilocybin shimmer! </t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/91ttzzhvm8pd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1fig9eb</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>Y’all weren’t kidding about cock a doodle doom…</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/12w3hk1nm8pd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1fifyza</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>Why does this remind me of sunscreen nails</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fifyza</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1fifmf5</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Clionadh GWP Flamingo </t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/m3lzpm08i8pd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1fiff5x</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>A moody skittle from ILNP’s Overcast Collection ⚡️☔️⛈️</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fifdzh</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1fieo80</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>Gentleman Pirate Appreciation Club</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h5059tqib8pd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1fiee4u</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Femme Fatale Wolfies </t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fiee4u</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1fiea71</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>Swift and Saddled… 5 different ways 😏</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fiea71</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1fie8ig</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>Nailpolish this shade that isnt Gel recs?</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mdmxcibd88pd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1fie0am</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>Perfect Halloween mani! Plus I love the name 😂</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fie0am</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1fidxcs</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>Mid Autumn Festival Nail Art</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/virncul468pd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1fidsm7</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The post from the other day got its own comic strip </t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yghqfyrjr5pd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1fidhuy</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>This polish is the prettiest copper with pink shimmer in it! I wish the camera picked it up better ):</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vhfle9gz28pd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1fidecy</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>I finally mastered the monarch wing trend!!</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w4y14ae928pd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1fidcka</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t xml:space="preserve">closest to neutral I’ve done in a while 🤣 </t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fidcka</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1fid7fj</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Obsessed doesn’t even begin to describe it!! </t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/b3p0l60v08pd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1fickbk</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>Nail art help!</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d9q3gpedw7pd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1fibwwo</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>Beetle wings 🪲</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fibwwo</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1fib57b</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>(Probably) Oxidized Chanel Rose Confidentiel :( lovely while it lasted</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/70nygns2m7pd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1fiar85</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>It’s fall and yall know what that means… SUPERSHORTIES RISE UP</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fiar85</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1fiaqa1</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Normal nail polish with uv? </t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fiaqa1/normal_nail_polish_with_uv/</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1fiaps7</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New collection shade name reveal! </t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fi5r1r</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1fiah4l</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Update on that $2 Walmart polish: my “too much gene” got the best of me 😂 Did I ruin the mani?! </t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zsb8crh5h7pd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1fi9vkj</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>Nothing There, by EDM, the perfect pale pink!</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fi9vkj</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1fi9e6s</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>Why are we doing aura nails?</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fi9e6s/why_are_we_doing_aura_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1fi9e4x</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>The perfect shade to transition from summer to fall. 🍂</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fi9e4x</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1fi97vo</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>Moody Nail Pish Recommendations UPDATE</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fi97vo</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1fi8vsk</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>The non-purple polishes in my collection are just for decoration</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fi8vsk</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1fi7wj6</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>Looking for something similar to KBShimmer Mull It Over</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fi7wj6/looking_for_something_similar_to_kbshimmer_mull/</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1fi7jed</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>A Forgotten Springtime Mani</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/o1n1x7sjw6pd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1fi7igg</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The Foxhole Court </t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fi7igg</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1fi6twf</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Like sunset in a bottle </t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fi6twf</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1fi6n4s</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>The magnet is worth the hype feat ILNP Deep Space</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fi6n4s</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1fi6fb1</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>Formulas like Mooncat?</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fi6fb1/formulas_like_mooncat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1fi6c1e</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>forest fairy 🧚</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fi6c1e/forest_fairy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1fi6a7m</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>ILNP Black Orchid on square shorties</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fi6a7m</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1fi601o</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gloomy day polish </t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s304oebcl6pd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1fi5u7s</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>it’s cold outside. 🍁🍂✨</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gupmhq05k6pd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1fi52yi</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>Cirque Lucky Jelly</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fi52yi</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1fi2lbw</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>Little messy but the first time I had a successful white!</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fi2lbw</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1fi0rhr</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fi0rhr/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1firjfv</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>Reverse-stamped flower nails</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1firjfv</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1fipis8</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>A Lil messed up</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fipis8</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1fiohbx</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>🩵FROSTED FLOWER NAILS</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/r9y7be2reapd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1finpgx</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t xml:space="preserve">loving how my “natural” raptor claws turned out </t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p072mcw68apd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1filaye</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Beetlejuice Beetlejuice </t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1filaye</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1fifkqr</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>Does anyone know how to achieve this "bubbly" texture</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fifkqr</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1fifb05</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>Nearly finished my beetlejuice nail set! 🥳 Here is Bob! He's my fav 🥰💕 Hand painted on 10XL cover tips 🤩</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/380vr9fzf8pd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1fieznz</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>twilight sparkle themed nails.. kinda</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fieznz</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1fidxqo</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Who’s ready for Halloween 🎃 </t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r75szti768pd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1fidvm3</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>Not A.I. just a really good photo😂</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v34spy4s58pd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1fidu2m</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>Bendy💅🏻</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/56u1nzgg58pd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1fid624</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Press on nailart learning to be a professional </t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3l54f49n08pd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1ficlns</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails inspired by Chappel Roans VMA performance </t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f48f2b2nw7pd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1ficbal</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Some practice for fall. </t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/il8lpenju7pd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1fic4p2</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>Lemon nails for my Mallorca trip 💛</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fic4p2</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1fiaekl</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love to create free style </t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/e5cyocoeg7pd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1fi9ekl</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Looking for color suggestions </t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1fi9ekl/looking_for_color_suggestions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1fi7qcs</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My nails expert is the best in Colombia. By Evelyn Mejía </t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tawaacjzx6pd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1fi615s</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>Mom Just Turned 77. Her Birthday Nails ☺️</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9sxrlf0kl6pd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1fi1b4w</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>Nails my friend made</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vge77s8mg5pd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1fhzizq</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>Freehand blooming gel art 💅🏻</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8b0bgd54t4pd1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Sep 18 08:10:34 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_09_22.xlsx
+++ b/data/collected_data/2024_09_22.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C491"/>
+  <dimension ref="A1:C661"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8780,6 +8780,2896 @@
         </is>
       </c>
     </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1fjnjnd</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>What’s the best shape for my nails?</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fjnjnd</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1fjmgdi</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Really damaged nails/nail beds. </t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fjmgdi/really_damaged_nailsnail_beds/</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1fjn74j</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t xml:space="preserve">These nails are so cute, but I can see Chiikawa disappearing on the first day. Inspo by @nailjolly on IG </t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7zghpkw2tipd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1fjmuow</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>I’m doing a French tip portfolio for the foreseeable future (vid contains July Aug Sep)</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/20dang5ooipd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1fjlnjh</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>Freshies 💙</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3nmiztqt9ipd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1fjlk6d</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mothman Nails </t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3mmkwu8q8ipd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1fjk6et</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>I love them!♡</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fjk6et</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1fjjm39</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>Smiley Faces</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nm1dyz7unhpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1fjh94m</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>Dip or gel?</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fjh94m/dip_or_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1fjfepb</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>Wedding nails suggestion</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8y21tnj5ngpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1fjj8a3</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>fresh set</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fjj8a3</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1fjirg1</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>Repost because I didn’t add the pic of them glowing in the dark!! 💚👻</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fjirg1</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1fji8el</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>My nails in different lighting 🥰</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fji8el</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1fjhvc8</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>Cut and file gel x??</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/35xij19t7hpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1fjhsds</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>Dipping into spooky season 👻</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e8lxejg27hpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1fjg0qu</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>What nail shape and color should I get to contemplate my engagement rings?</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fjg0qu</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1fjgr6z</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>Sabrina Carpenter Inspired Nails</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fw4eqqkyxgpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1fjh555</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Haters said Japanese manicure damages your nails. I’ve been doing it for 4 months and my nails are healthier than ever. </t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2obfd37a1hpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1fjgrcn</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>Pic from a few weeks ago but I really loved this color</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sb75nm2zxgpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1fjgo5w</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>Which shape suits me the best?</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fjgo5w</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1fjgjjp</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>Advent calendars?</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fjgjjp/advent_calendars/</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1fjft9j</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>Update: Thanks for helping me pick my dip manicure!</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fjft9j</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1fjfsyo</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Edlen Tonic Photoshop </t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/773r6ai8qgpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1fjfi4z</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>What colour nails for my son’s baptism?</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gsoert5wngpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1fjbpkn</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>Update: Thanks for helping me pick my dip manicure!</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fjbpkn</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1fjcjnf</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>polygel recommendations for a beginner?</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fjcjnf/polygel_recommendations_for_a_beginner/</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1fjeqox</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>Lord of the Rings inspired</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fjeqox</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1fjf109</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Advice? </t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/shjl0hd5kgpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1fje66m</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>really tight c curve nails!</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fje66m</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1fje1a4</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>Dip Vs gel for colors?</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fje1a4/dip_vs_gel_for_colors/</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1fjdiki</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Berry teal shift </t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/cqkqyg9n8gpd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1fjd6dj</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>best manicure for a surfer?</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fjd6dj/best_manicure_for_a_surfer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1fjcxhu</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t xml:space="preserve">When to apply oil? </t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fjcxhu/when_to_apply_oil/</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1fjcweb</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I’m obsessed with long nails </t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fjcweb</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1fjcmbe</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>First time</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w7nlyo2z1gpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1fjbkh8</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>My 1st ever nail extensions</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fjbkh8</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1fjc929</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>New nails today</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3jz2r4n9zfpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1fjbjoc</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t xml:space="preserve">January Vs Now </t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fjbjoc</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1fjbja8</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>Builder top coat on tip of normal gel polish?</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fjbja8/builder_top_coat_on_tip_of_normal_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1fjafk8</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>2 year progress</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fjafk8</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1fjalbm</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>Green green☘️</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fjalbm</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1fj7ngi</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>Is it too soon to get my nails redone?</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fj7ngi/is_it_too_soon_to_get_my_nails_redone/</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1fja4tq</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ocean nail set I came up with! </t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hlw3bq3fkfpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1fja3gu</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>A set I free styled!</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q0e8qm66kfpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1fj21hq</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>Coraline inspired nails 🪡🧵</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fj21hq</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1fj9l57</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time hand painting my French tips on. </t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fj9l57</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1fj99gx</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> cuties, what do you think about the colour? ✨🥰</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/27bdfpueefpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1fj8p08</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New fall nails </t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fj8p08</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1fj8onc</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I have been growing my nails out but I don’t want them to look unclean. I have a nail brush and applied the Sally Hansen nail hardener. Do they look ok? Should I try another shape? Any advice is appreciated! </t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fj8onc</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1fj8oh3</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My first Halloween set of the season </t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0is7kieeafpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1fj753l</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Loving the way these BIAB nails complement my skin tone. 🌸✨ </t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ljcrwpvpzepd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1fj74s4</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I gave myself all the sparkles today </t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wdih3h4rzepd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1fj74is</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>In between seasons...☀️🍎🍂</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wor5wzvpzepd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1fj49ib</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>Where to start with Press Ons?</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fj49ib/where_to_start_with_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1fj6qya</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>First time getting acrylics</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fj6qya/first_time_getting_acrylics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1fj6cgn</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>Glow in the dark🖤</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fj6cgn</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1fj5mzu</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>Earth Tones 🌍🌱</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hc0fd6e7pepd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1fj53ho</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>Practicing my shapes for school! 💕</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fj53ho</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1fj4b94</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>Do these look decent ?</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vlftu4m7gepd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1fj4b38</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>💘💘💘</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tnou1wc7gepd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1fj43hm</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What are “oil based” nail polishes &amp; how are they different to Essie/Revlon etc </t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0tjb5ygreepd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1fj3mlr</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>looking for an apron</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fj3mlr/looking_for_an_apron/</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1fj2x1h</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>What’s a gel polish close to this color?</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5s4eor3o6epd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1fj2q2y</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Feeling extra cute with my froggy nails! </t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/74spkly85epd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1fj2fsb</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I think this the best set I have ever done so far 🖤 </t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fj2fsb</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1fj1o5i</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>Glazed donut nails on my sister to get ready for fall 🍩🍂</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fj1o5i</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1fj18vd</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hawaiian 🌺 </t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9cjrtcvnudpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1fj0yrt</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>Got nails done for my 30th birthday</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/alxvr25nsdpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1fj06co</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>I’m calling these “Island Fall”!</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ubv2x2csmdpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1fizkue</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>Me in my clean girl phase 🤗</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l0304acbidpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1fizby5</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>Butterfly nails!</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fizby5</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1fiz2sb</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t xml:space="preserve">showing off my warm season nails 💅🏼 </t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jcg3un4gedpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1fiy8zv</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>Bordeaux this time 🍷🍂♥️</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m62pkiz28dpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1fixit3</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Once again, the glitter gods have spoken to me. By far my favorite one yet! </t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fixit3</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1fiptvx</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>Madam Glam - when do they restock?</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fiptvx/madam_glam_when_do_they_restock/</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1fiwd16</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>Digging Matte on this Style</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/udg86ufjrcpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1fiw9v9</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>Flaunting the Pride 💜</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ajaj16wnqcpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1fiv0bd</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>I want your honest advice on the second set of nails I’ve done 💅</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/addwehvddcpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1fiudjq</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t xml:space="preserve">how to regrow nail bed? </t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fiudjq/how_to_regrow_nail_bed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1fitw7a</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>Fall nails (my first ever set of acrylics)</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fitw7a</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1fit461</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>I love long nails, what do you think?</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mhabucjrqbpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1fisxy7</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>Which nail shape?</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fisxy7</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1fjlzd4</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>Garden Path Lacquer I Forgive You 🪴✨</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fjlzd4</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1fjlq6o</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>I got my order today! Tell me which one I should use first. ❤️🖤🩷</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fjlq6o</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1fjlnxc</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>final summer manu of the year</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fjlnxc</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1fjlbqe</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>my nails were sun kissed</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v0vyfh6u5ipd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1fjkux9</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>Favorite oranges?</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fjkux9/favorite_oranges/</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1fjkp8o</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>Just used gel polish for the first time ✨</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0tet1aazyhpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1fjjnv1</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>Fae or Fomo?</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fjjnv1</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1fjj1nj</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>I think I found gold</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fjj1nj</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1fjhnap</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>First time trying pearlescent polish!</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fjhnap</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1fjf1ra</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>Holo saves shitty black polish!</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fjf1ra</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1fjeyuc</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>X-Men Nightcrawler nail art 💙🖤</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fjeyuc</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1fjeszz</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>Wearing Tuesday the 17th, on Tuesday the 17th, while watching Tuesday the 17th 🩷🍍🩷</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uuslj8qdigpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1fjelj0</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Need help choosing nail color to go with burnt orange dress! </t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q15jzdutggpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1fjehzn</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>lights lacquer - scorpio</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wr7ea5v2ggpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1fjeb52</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>BCB Lacquer "Love at First Bite" (Halloween 2024 Advent day 8)</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fjeb52/bcb_lacquer_love_at_first_bite_halloween_2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1fjd7ws</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>Alien Infatuation ✨️👽</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/up0li7hf6gpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1fjcula</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Show me your Fall brown manicures! </t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fjcula</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1fjcsd8</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>three coats of polish (somehow)</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7eijmaj73gpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1fjclq6</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>replacement caps/brushes for ILNP</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fjclq6/replacement_capsbrushes_for_ilnp/</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1fjcdb0</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>Why does this happen? The bubbles in the nail polish drive me crazy. I thought it was because of old nail polish, but this is a brand new nail polish</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qv80xi940gpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1fjc5rd</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>What is your go-to polish remover?</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fjc5rd/what_is_your_goto_polish_remover/</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1fjbor1</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>Has anyone tried Zoya’s “Ultra Glossy Seal Top Coat”?</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fjbor1/has_anyone_tried_zoyas_ultra_glossy_seal_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1fjbnip</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>Pick tonight’s polish for me?🎲</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iqtnbh11vfpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1fjb698</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>Doing nail art after a yearlong break🥲</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d58hvnh2rfpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1fjb306</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>Rejoining team shortie</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fjb306</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1fjaot5</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>Embracing my super shorties</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fjaot5</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1fja01r</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>info about lights lacquer</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fja01r/info_about_lights_lacquer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1fj8iw4</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>IDK When It Happened, How It Happened, Nor Why It Didn’t Hurt But RIP To My Fingernail</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9nvzq2cb9fpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1fj7w78</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Are my nails too damaged for press-ons? 🫠 </t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3rbszymx4fpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1fj7foa</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>Fave fall combo</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/va527cnv1fpd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1fj773r</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t xml:space="preserve">fall nails!!! 💅 </t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fj773r</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1fj76xe</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Spotted nail polish </t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fj76xe/spotted_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1fj6zta</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>Mooncat Recommendations?</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fj6zta/mooncat_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1fj6mrn</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gir! </t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fj6mrn</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1fj652j</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>What is the last product that you purchased due to this sub and what did you think of it? - Laqueristas Edition</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fj652j/what_is_the_last_product_that_you_purchased_due/</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1fj4zcp</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Need recommendations for a good quality, affordable base coat and top coat! </t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fj4zcp/need_recommendations_for_a_good_quality/</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1fj4o46</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>Just a bit of happy on an otherwise bummer of a day</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ymxlflxniepd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1fj4ff6</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>By Dany Vianna- Evangeline</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rn30upn1hepd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1fj48i0</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>Mooncat - Merkitten :)</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fj464q</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1fj47e1</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>✨️🌈Rainbow Sparkle🌈✨️</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fj47e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1fj3y7y</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>Obsessed with the shifts in the morning sunlight.</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6l8fm3lidepd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1fj3r4v</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>scorched earth appreciation 🔥✨</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fj3r4v</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1fj3e4l</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>ILNP “Misty” aka the perfect flake lavender</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fj3e4l</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1fj3cyx</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>Magnetic polish on press ons?</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fj3cyx/magnetic_polish_on_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1fj2vut</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>I’ve never worn “brown” polishes before. Holo Cappucino by Holo Taco though?? I’m in LOVE</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fj2vut</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1fj2tkp</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>Makers who post behind the scenes?</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fj2tkp/makers_who_post_behind_the_scenes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1fj1eqg</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>Nail stickers Amazon vs SHEIN</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fj1eqg/nail_stickers_amazon_vs_shein/</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1fj0xoh</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>First time using nail stickers! Cat tax included (her name is Skunk)</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fj0xoh</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1fj0xd8</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>All new manicures must be approved by The Polish Inspector</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fj0xd8</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1fj0ks8</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>Magenta</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/hCrD58f</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1fj0dd8</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>hi. 🌑🍁🧚🏽‍♀️✨</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vnyabcg9odpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1fj09cs</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>ILNP After Hours is the most beautiful, shifty, magnetic polish I have ever seen!!</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/IJrRdnr</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1fj08od</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>Does an extended time between base coat and paint matter?</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fj08od/does_an_extended_time_between_base_coat_and_paint/</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1fizzpr</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>Zoya 5 for $25 sale (ending 9/20)</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fizzpr/zoya_5_for_25_sale_ending_920/</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1fiztbm</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>Black polish with gold/bronze/copper shimmer/flakes?</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fiztbm/black_polish_with_goldbronzecopper_shimmerflakes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1fizn84</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My dad built me a display rack! </t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1454h3ctidpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1fizh9o</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Something special happened this weekend! This polish now has a special place in my collection. </t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qkv9d9fjhdpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1fizawg</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A glowing Cosmic Cowboy </t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fizawg</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1fiz2z7</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>Have you ever wondered what happens when a bottle of nail polish goes through the dryer and the bottle opens? No? Well, I answered the question anyway!</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6yskmlnhedpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1fiywtm</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>Anyone know where I can find these polishes in Canada?</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kz5rmma6ddpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1fixt1z</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mac - Formidable! Beautiful in the bottle, a pain to get on your nails </t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fhs9u3</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1fiwxu1</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>My nails have been peeling for the past 5 months. Please read text and help me make judgement</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fiwxu1</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1fiws2k</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>Has anyone ever made their own nail polish?</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fiws2k/has_anyone_ever_made_their_own_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1fjljp2</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>Those of you who use press on nails. What glue do you use that can withstand doing dishes, housework etc…?</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1fjljp2/those_of_you_who_use_press_on_nails_what_glue_do/</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1fjl5s7</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>Fluid nail art! Can't stop staring!</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fjl5s7</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1fjl3mo</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Beach themed press ons </t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fjl3mo</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1fjki74</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>Fall nails 🍂🍁</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c7qh7gltwhpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1fjitmp</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>Just look at this beauty</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9igf8audghpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1fjisvb</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>I was 10 years old again</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jrllscq6ghpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1fjh7sr</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>Beetlejuice Nails</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pvhbnq2z1hpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1fjh721</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>Hyper-contemporary</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/td052m3s1hpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1fjcdov</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>Birthday frosting play on French tips</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/poxbyc370gpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1fja1d9</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My new nails </t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z0l8zzbrjfpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1fj8l2z</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>I am obsessed with the glass artist Treyjane’s glass nails.</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://m.youtube.com/shorts/0LUSaDvpqkg</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1fj85gd</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>Spooky halloween set I just finished for myself 🎃</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fj85gd</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1fj5sey</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>Picnics</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fj5sey</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1fj5qqf</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>Fruit nails</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p2ppvbrwpepd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1fj51vv</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>Tortoise Shell Design</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zussdgg9lepd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1fj4r74</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>My own press ons 🫶🏼</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fj4r74</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1fj4fzo</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>Clouds and Glitter</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jq6bxgv5hepd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1fj49w4</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>Do you remember where you've seen this haunted house before? Say hello to our little Pumpkin and Mummy! 🎃👻</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5dpo8skqfepd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1fj3eha</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>My flowers came out so cute. 🥹✨</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/in8arlj0aepd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1fj1x1r</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>How much should I expect to pay for these nails?</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/chk3cejhzdpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1fiya4r</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>Bloody Romance Vampire Nails</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/b2uqgv198dpd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1fiy3p3</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Beetlejuice inspired nails. </t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kpphvlby6dpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1fiwdvr</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>Love this set</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vcapwwwrrcpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1fivn5m</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>The Detail!</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fivn5m</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1fitp0t</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>Ladybug Nails</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fitp0t</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Sep 19 08:11:14 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_09_22.xlsx
+++ b/data/collected_data/2024_09_22.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C661"/>
+  <dimension ref="A1:C867"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11670,6 +11670,3508 @@
         </is>
       </c>
     </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1fkeybd</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Looking for 420 ladies with elaborate nails?? </t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fkeybd/looking_for_420_ladies_with_elaborate_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1fkewm4</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Any comments on the colour? </t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0arbbthdtppd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1fkevx5</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>do they look awful?</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fjb1jw04tppd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1fkeoex</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>Curved toenails from pedi?</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/51rl94bbqppd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1fke2lr</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>Small chip fresh gels</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fke2lr/small_chip_fresh_gels/</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1fkdyd6</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t xml:space="preserve">These are my civil wedding nails </t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fkdyd6</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1fkdtkf</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>It’s fall time🍂 obsessed with this</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fkdtkf</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1fkbunz</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I painted Lydia! Still working on my beetlejuice set only one more to go! (These are NOT meant for daily wear y'all it's art/fun) </t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/li2pqgiptopd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1fkax15</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>Can anyone help me find a dark olive green gel polish in this range?</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/CWoeCKT</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1fkas3u</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Girls day nails </t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fkas3u</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1fkd4r8</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>Summer white Swirl French design</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bl44t0iw6ppd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1fk8o5r</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>Can anyone whos used both tell me which is better?</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fk8o5r/can_anyone_whos_used_both_tell_me_which_is_better/</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1fkczq9</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>First time getting cat eye and I’m obsessed</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fkczq9</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1fkcvsr</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>snapped my thumbnail off in the car door. i scrum so fkin loud</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lycf0jqo4ppd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1fkcsdm</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Only had them for a week </t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qr2dgcnn3ppd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1fkcr8p</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>♥️</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/61f0e0wa3ppd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1fkcctq</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t xml:space="preserve">please help </t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fkcctq/please_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1fkc7ru</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t xml:space="preserve">OPI Gel Equivalents </t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fkc7ru/opi_gel_equivalents/</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1fkbvml</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>Hello kitty sugar frenchies🎀</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/10ekjryytopd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1fkbrai</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>Kirby Press Ons I Made!</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fkbrai</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1fkbr77</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Y'all! </t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fkbr77</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1fkbqdt</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>September nails</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fkbqdt</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1fkbaqk</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>My first set of Halloween nails for this year 👻🩷</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fkbaqk</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1fkb6tp</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pink💖 </t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8mhl07g1nopd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1fkb0ks</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I switched to Apres Gel-X recently and I am obsessed. </t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fkb0ks</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1fkaz7v</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>Tried a new nail tech. Do we like? 🤩💚</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fkaz7v</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1fkarh4</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>Blueberry Lemonade Anyone?</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qv4fgjvziopd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1fkafcq</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>Are these as bad as they seem?</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fkafcq</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1fk9r3z</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>I love this natural color. You can't see the cat eye but it's beautiful.</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tx3u8k8t9opd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1fk9dbx</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>Update: I took your suggestions and tried filing them to almond shape. Do they look a little vampire-y or am I just not used to it? Advice appreciated, thank you!</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tp3kuwhe6opd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1fk992o</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>Made myself some Strawberry Shortcake 🍓💖</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/r2bz5vr55opd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1fk90j8</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>My take took his time...?</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8osxpkd83opd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1fk8k0q</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>Matte top coat on top of a magnetic polish</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fk8k0q</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1fk87vb</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>Super opulent charm bracelet nails by me 👑</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fk87vb</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1fk7iee</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Looking for a gel polish dupe of Huey from Don Deeva </t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/odumndpwpnpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1fk7i7l</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>Gel X to Acrylic?</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fk7i7l/gel_x_to_acrylic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1fk7h8q</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Impressed with my imPress </t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fk7h8q</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1fk7ef3</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>before and after some colour and chrome</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fk7ef3</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1fk7d2m</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>my current set ❤️</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uks69l6ronpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1fk6lxj</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BTArtbox top coat peeling. What am I doing wrong? </t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fk6lxj/btartbox_top_coat_peeling_what_am_i_doing_wrong/</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1fk6hno</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>Excited about my current nails ☺️😍😳 It’s my second time having acrylics 🙂</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fk6hno</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1fk69w6</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>French ballerina press-on, what do you think?</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/bl9TwPU</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1fk69fd</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>Thoughts on this color?</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ymw0diygfnpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1fk68b0</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>Tested out my new gel. How did it come out?</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fk68b0</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1fk5lk2</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>Need Advice for Durable Fingernail Polish or other Products</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fk5lk2/need_advice_for_durable_fingernail_polish_or/</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1fk5gxl</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>One month of biab and I’m so happy these are my own nails!</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9lb1cx8s8npd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1fk5ftg</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Olive 🫒 for fall </t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3lz23dzi8npd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1fk56cj</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>Very cutesy, very (not) demure</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/do7036jf6npd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1fk4rei</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>Help ID'ing please?</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/orgyr1b43npd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1fk49xp</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>Gel X lifting at base</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1mmnsbc9zmpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1fk44hn</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pink chrome french </t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b9bz3nc1ympd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1fk3ebn</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>Falllll🍂🍁🎃</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kf0jcz6ismpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1fk2ut6</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>Ready for Fall 🍂🍁</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fk2ut6</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1fk2omm</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>Acrylgel extension Q</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fk2omm</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1fk2h19</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>First ever set I've done!</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fk2h19</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1fk2gqu</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Did my nails for the first time in a while </t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fk2gqu</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1fk20xw</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Girly on Reddit saw my work and was in my area so I did her nails❤️ my first real client set </t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fk20xw</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1fk1y5e</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>birthday nails ideas?</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fk1y5e/birthday_nails_ideas/</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1fk1w84</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>...whoops</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c0zm9lgchmpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1fk1tp3</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>I’m loving this dip mani 🥰</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e0o429atgmpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1fk1rjy</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>Does this colour look dull on me?</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/shyqnhwbgmpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1fk0bd8</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>Which nail glue should I purchase for super extra long-lasting results?</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jqj9j44b5mpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1fk1o8g</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>What are your thoughts about my nails 😙</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fk1o8g</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1fk1b9b</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>Did my own nails with hard gel</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fk1b9b</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1fk18u1</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Need hello locating vintage polish! </t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fk18u1/need_hello_locating_vintage_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1fk143t</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>Vacation nails</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fk143t</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1fk0wfv</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>Framed fungi 🍄‍🟫</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s160tzjs9mpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1fk0qye</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>today's nails! tips and semi enamelled💋🤩</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/10a8k5bl8mpd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1fk0mf8</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>Not a professional just a girlie with a hobby 👉🏻👈🏻</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nuy82f7n7mpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1fk0m5r</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>My Nail Designs</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fk0m5r</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1fk0dra</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>Shout out to Kashalein for the inspiration (last picture). Fresh, clean and neutral for fall 💜</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fk0dra</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1fjzxfh</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>So jealous</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g9k29bnd2mpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1fjzwvh</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>Preston's or acrylic? (Ignore the my hand)</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ny444hf92mpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1fjzw6j</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>New press ons 🥰🖤💀</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fjzw6j</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1fjyykk</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>Polygel keeps lifting</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fjyykk/polygel_keeps_lifting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1fjyyjj</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>Clean girl aesthetic</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x5ag3kt2vlpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1fjyxmv</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>Evergreen ❤️</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kobwu5fwulpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1fjyuq6</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>Love the colour and flowers on these new nails</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fjyuq6</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1fjymmh</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>DIY Builder Gel Sets!</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fjymmh</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1fjy7ai</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>Raptor claws</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fjy7ai</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1fjy59z</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>Ghostface nails 👻</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fjy59z</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1fjthni</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New 💅 </t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fjthni</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1fjxpvy</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The best set I have ever chosen! </t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ns9y16arllpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1fjxo35</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>My last few sets, love my nail tech's work!</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fjxo35</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1fjq8sc</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New set or not bother? </t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fjq8sc</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1fjqdka</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>Is it really that difficult/unsafe to do your nails at home?</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fjqdka/is_it_really_that_difficultunsafe_to_do_your/</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1fjx5br</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>Nails ive done recently :)</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fjx5br</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1fjwuxt</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>So it begins!</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fjwuxt</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1fjxjv2</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails never last </t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fjxjv2/nails_never_last/</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1fjxjiy</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>Searching for a gel nail polish brand!</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fjxjiy/searching_for_a_gel_nail_polish_brand/</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1fjw346</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>Spooky season nail inspo</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8tlok9eo9lpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1fjvybv</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>I got my nails done today what do you think</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fjvybv</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1fjv2ky</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>Can someone explain different types of press ons? Looking at BTartbox</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fjv2ky/can_someone_explain_different_types_of_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1fjteao</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>pink? pink! (second time painting these :3)</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ikyxzacipkpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1fjpwrv</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>Freehand gold fish💗</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nn1i24ggtjpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1fjprqh</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>Short press on almond nails</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fjprqh/short_press_on_almond_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1fjwalo</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gel Builder 1st Timer </t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fjwalo</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1fjw99n</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>Gel polish bad for toes in the winter?</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fjw99n/gel_polish_bad_for_toes_in_the_winter/</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1fjw8gr</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>first time doing ombré french dip nails 🩰</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fjw8gr</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1fjms5m</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>Ocean inspired abstract French I made on my friend for her holiday ☀️</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/esx7jzosnipd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1fkcur3</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>Loving jelly sandwiches this spring</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fkcur3</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1fkby1p</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>ILNP Starlight ✨</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8gw1zkjouopd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1fkbkr6</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>The perfect artichoke</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fkbkr6</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1fkbads</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>which type of nail polish/gel/acrylic/etc is best for ur nails?</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kgleqlg0oopd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1fkb4v3</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>Hi, I'm new to painting my nails as a 28 year old lol, can someone tell me how close these shades are? (details in comments)</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://i.imgur.com/nqQk0bV.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1fk9szb</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>What polish with this dress?</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6piv27lbaopd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1fk9qvq</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Psilocybin 🍄 </t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vjs1go9r9opd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1fk9cto</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>Don’t sleep on Hot Topic polish!</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fk9cto</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1fk8qkh</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>“Boho Chic” from Fancy Gloss, Thermal + Holo</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fk8qkh</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1fk8mwl</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>Matte top coat on top of a magnetic polish</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fk8mwl</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1fk8gxm</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>Cadillacquer- Many Moons</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wc4v3yuaynpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1fk7iab</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>Kur Nail Concealer</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fk7iab/kur_nail_concealer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1fk7eks</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>revlon spidey sense dupe</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5yvviz25pnpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1fk7832</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>First ever dip and I'm IN LOVE!</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fk7832</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1fk75gx</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>What brands are worth it?</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fk75gx/what_brands_are_worth_it/</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1fk6wvj</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>Last summer nail color of the year!</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tigqjdixknpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1fk6n1o</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>Anyone know if Orly will bring back their glow in the dark toppers? (+ GITD recs?)</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fk6n1o/anyone_know_if_orly_will_bring_back_their_glow_in/</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1fk6dpk</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>♥️✨</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fd29j6fhgnpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1fk62c3</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>Longest my natural nails have ever been (I’m now a FORMER nail biter thanks to this sub!) &amp; first time painting my own nails in years 🧡🎃</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kp2c4matdnpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1fk5x85</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>LA colors Jelly sheer</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f8l1rsmlcnpd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1fk5cqt</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>swatched all the polishes I’ve gotten since last year!</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fk5cqt</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1fk4dg4</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>Lemming</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fk4dg4/lemming/</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1fk4brd</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t xml:space="preserve">More clionadh magic </t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fk4brd</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1fjhdr6</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>This week’s color!! I’m loving it</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fjhdr6</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1fk41yc</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>Fall campfire mani</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qny9g6xhxmpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1fk3rd7</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Long time reader, first time poster </t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fk3rd7</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1fk3fp0</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>ILNP - Cameo (pink to green multi-chrome)</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fk3f3q</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1fk3clp</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>Extension Shaping Question</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fk3clp</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1fk3a66</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>Fall skittle!</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fk3a66</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1fk34x5</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>Sheer red polishes that aren't too magenta?</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fk34x5/sheer_red_polishes_that_arent_too_magenta/</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1fk2flv</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>My new favorite thing</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4ldrzhk8lmpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1fk288f</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>Should I put an overlay over my nails or leave them be?</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/z3rdcb4qjmpd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1fj9lft</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gel Allergy Alternatives </t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fj9lft/gel_allergy_alternatives/</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1fjc3a1</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>Eclipse for tonight’s lunar eclipse/supermoon 🩸🌔</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fjc3a1</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1fjfhcp</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>Overfiled at salon but wedding is in a few days</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fjfhcp</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1fjv2fb</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t xml:space="preserve">HELP!!! top coat peeling </t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fjv2fb/help_top_coat_peeling/</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1fk1vwy</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>First time trying Emily de Molly</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fk1vwy</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1fk1vv5</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t xml:space="preserve">hot gossip ! </t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fk1vv5</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1fk1f7g</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>September drops?</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fk1f7g/september_drops/</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1fk0j0g</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The ✨I’ve discovered pretty polish✨ haul </t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fk0j0g</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1fk0d8f</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>Round 2 of the creme challenge (aka how long until I add glitter?)</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ur3apfo5mpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1fjzm4s</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>Pain with nail growth?</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ds4fd4o00mpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1fjzjjn</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>Finally had the energy to make them all nice and shiny :)</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ivi3yonhzlpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1fjys3q</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>🩵🧡Mid-Century Modern🧡🩵</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fjys3q</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1fjyrpc</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>👀 New Brand?! Prism Parade launching this Friday!</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fjyrpc</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1fjygf5</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t xml:space="preserve">feeling blue </t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e85efml9rlpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1fjy5ff</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>Favorite Seche Vite alternatives?</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fjy5ff/favorite_seche_vite_alternatives/</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1fjxird</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>Nail care Help</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/udoy5ct8klpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1fjxbil</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>Eben Ice Caves - LynBDesigns</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fl16xu2silpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1fjx8qv</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>Simple nail art ideas to enhance a pinky-nude linear holo?</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mz1bt9f7ilpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1fjx83n</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>JL Lacquer Manoa</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dow2b7r2ilpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1fjx49c</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>Last ode to summer courtesy of cirque</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ltjfafy9hlpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1fjx0zq</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>Finally got a 30lb horseshoe!</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/56ychzwgglpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1fjwvkm</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Black with pink/fuchsia glitter?  </t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fjwvkm</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1fjvkr9</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>Addiction Tokyo polishes?</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fjvkr9/addiction_tokyo_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1fjua9b</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Electric orange </t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fjua9b</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1fjsz9s</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>Stamping Polish Recs Please</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fjsz9s/stamping_polish_recs_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1fjsw9b</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Feeling like an Emerald Princess </t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fjsw9b</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1fjsg39</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>Matching Psilocybin to my dress!</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fjsg39</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1fjs2j6</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My wedding nails! </t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fjs2j6</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1fjrosq</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>Must-Have Zoya Shades?</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fjrosq/musthave_zoya_shades/</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1fjqj6j</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>Favorite Pink Shimmers 🩷</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fjqj6j</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1fjqbax</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>PSA to all who were looking for Chanel Phénomène!</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fjqbax/psa_to_all_who_were_looking_for_chanel_phénomène/</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1fjocvd</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>What to use to clean nails</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fjocvd/what_to_use_to_clean_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1fj5cn1</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>Any shops in los angeles that sell chrome powders?</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fj5cn1/any_shops_in_los_angeles_that_sell_chrome_powders/</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1fj58ca</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>looking for a solid builder gel that can soak off</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fj58ca/looking_for_a_solid_builder_gel_that_can_soak_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1fkf60w</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>3D acrylic.  Is it giving Halloween vibes?</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fkf60w</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1fkevcb</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Homecoming nails for my sister </t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fkevcb</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1fkerrv</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>my first ever nails (any tips on how to get better?)</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hp5hsq7mrppd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1fkcq5k</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>🤍✨</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vjnuemcz2ppd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1fkc033</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>Black to colourless/clear thermal gel</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1fkc033/black_to_colourlessclear_thermal_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1fkbrfv</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I painted Lydia! Still working on my beetlejuice set only one more to go! (These are NOT meant for daily wear y'all it's art/fun) </t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/pt4cayessopd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1fkbqv9</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>Kirby Press Ons I Made! Criticism is welcome</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fkbqv9</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1fkblw6</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>Tried alcohol inks for marbling💖💙💖</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wcr1iu97ropd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1fkbjev</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>This design is very Disney, what do you think of this length? 💅🏼❤️</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/caxws4uhqopd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1fkbhuz</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>Today I made this Halloween design, and I'm fascinated with this date 😍💅🏼</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9tfsyts1qopd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1fkbh21</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>I love it when they bring me daring things, what score do friends give it? 💅🏼💅🏼💅🏼❤️</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/670diodtpopd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1fkbgp7</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>does anyone have any tips to not make the designs look lumpy like this?</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vsa0l8zppopd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1fkbg8e</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>My girls have the best designs, what score do they give from 1 to 10? 💅🏼💅🏼</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pjv5kdtlpopd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1fkaa01</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How did I do? </t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fkaa01</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1fk9g4s</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>Nightmare Before Christmas Nails!</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fk9g4s</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1fk8pqz</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Matte topcoat on magnetic polish </t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fk8pqz</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1fk897v</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>Super opulent charm bracelet nails by me 👑</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fk897v</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1fk7rti</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First try at tortoise nails </t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xrj08lcbsnpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1fk6dmg</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Vantablack Acrylic </t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l9g4fhsggnpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1fk69iy</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>On my 30th try I finally did it. Is it good girls? :)</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fk69iy</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1fk515r</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>TW:blood art</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wanqgg395npd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1fk4z5b</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>Crystalline🔮</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iuvnl61t4npd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1fk3guv</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>Cute lil fall nails🍂</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fk3guv</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1fk3gr1</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>Cute lil fall nails🍂</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fk3gr1</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1fk2hea</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>Pop like this Pt. 2 (Slowed)</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://youtube.com/source/QlpDZ0meV-Q/shorts?si=T_73ym-vRwS-5Age</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1fk2b56</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>Cubed</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/p5usdjtbkmpd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1fk0ryo</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>Sweets for my sweet</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fk0ryo</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1fk0qji</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>My first nail design:)</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/65mnk9xh8mpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1fk0k70</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Not quite fall but getting there </t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fk0k70</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1fjz9yt</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gems!💎 </t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fjz9yt</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1fjz786</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>Southwestern vibes</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fjz786</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1fju6g6</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Continued </t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fju6g6</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1fjtucj</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sweetie pie continues </t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fjtucj</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1fjtswy</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Continued nail art being inspired </t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fjtswy</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1fjq74l</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>This took me 4 hours to do... is it good? ;))</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wgzu0y5iwjpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1fjpt6w</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>My girlfriend did my homecoming nails!💜</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aho2m4l9sjpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1fjpijf</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sweet time </t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pvoxqxlsojpd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1fjoy5w</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>Sweetie pie should I continue</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8h2u0gtthjpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1fjoww4</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>Sweets for my sweet continue or not?</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/04v6uuxbhjpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1fjnv0m</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t xml:space="preserve">who likes mini eggs! </t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6emu7ehl2jpd1.png</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Sep 20 08:10:30 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_09_22.xlsx
+++ b/data/collected_data/2024_09_22.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C867"/>
+  <dimension ref="A1:C1046"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15172,6 +15172,3049 @@
         </is>
       </c>
     </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1fl6iz0</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>new set for my bday! 🤍</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fl6iz0</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1fl5sbg</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>Nails color</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lo8eia55uwpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1fl5602</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Before and After- 45 days growth </t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fl5602</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1fl47w4</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>First time trying Neon nails</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fl47w4</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1fl41ck</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>Embracing my natural nails</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/whlyiy4l8wpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1fl3uk9</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>How did I do? (First time)</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fl3uk9</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1fl3sem</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>Fall nails 🍂🍁</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h64qz7io5wpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1fl3ojh</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>Tips to get into doing my own nails</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fl3ojh/tips_to_get_into_doing_my_own_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1fl2iij</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>Update from last night!</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fl2iij</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1fl397b</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Did my friends nails part 2 </t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fl397b</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1fl33bt</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>New to visiting nail salon</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fl33bt/new_to_visiting_nail_salon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1fl2wg8</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails </t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fl2wg8</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1fl2lw1</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>{PR} Sassy Sauce | Wicked Sorcery</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fl2lw1</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1fl2l0o</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>Romantic Roccoco</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wzwby7w4tvpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1fl1vx4</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time drawing french tips by hand, how did I do? </t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fl1vx4</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1fl1sig</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>My nail polish gathers</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fl1sig/my_nail_polish_gathers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1fl1r7y</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t xml:space="preserve">💜💚 Beetlejuice 2 Duo, Painted Polish and Rogue Lacquer collab </t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fl1r7y</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1fl1q7w</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>Go back?</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fl1q7w</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1fl1opa</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t xml:space="preserve">long lasting manicure? </t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fl1opa/long_lasting_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1fl1guj</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>Natural Nails</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c0v8l9tfivpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1fl1ebf</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>still loving glazed donut ✨</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1x4rbfarhvpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1fl1ea2</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>still loving glazed donut ✨</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ebr8euyqhvpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1fktm5a</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>Nail inspo for Halloween</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fktm5a/nail_inspo_for_halloween/</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1fl0r1j</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>Made another press on set for a friend; this time Halloween themed!</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/syaqvjonbvpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1fl0g5f</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My spooky nails 💅🏾 🦇 </t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fl0g5f</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1fl06ta</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>Got a pedicure to match my manicure...I absolutely loveeeee how the color came out</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c8nioe0a6vpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1fkzvfu</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Trying to decide if I like them or not !        Opi love is in the 🐻 </t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vr4r9cke3vpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1fkzmzi</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Beetlejuice Press on Nails </t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fkzmzi</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1fkzl55</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Minecraft Nails </t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fkzl55</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1fkzgu1</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>I didn’t really think this through and now my nails are giving big Christmas vibes 🤣</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fkzgu1</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1fkzf7c</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>Set I did for Vegas!</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fkzf7c</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1fkzbw4</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>Pigment powders are too good at covering?</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fkzbw4/pigment_powders_are_too_good_at_covering/</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1fkyy8f</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>gel x nails</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fxcsehr0vupd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1fkywrn</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>Moderate delamination- to file or not to file?</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fkywrn/moderate_delamination_to_file_or_not_to_file/</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1fkysnf</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>So proud of this set!</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fkysnf</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1fky9l3</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>I am quite simple and basic but I love nails like this</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xk2jfv7youpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1fky4tv</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>Glass nails</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pbanfqxtnupd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1fkyiof</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>Love Easy Builder Gel</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bcgs2sc9rupd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1fkyczx</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>🐙</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9s7w3oxtpupd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1fkyb2w</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>Blueberry nails 🫐</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fkyb2w</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1fkyaw2</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>Mix match ❤️🤍🖤</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lcng35vapupd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1fky86q</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>ICP nails i did today!!!</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/lhoftz9noupd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1fkujuz</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>There's a Ghost in the Greenhouse: Gel X Art, first time</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fkujuz</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1fkvg81</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I’ve been growing my nails back to their claw status and am in love with this reptilian inspired manicure. </t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/brk0rcpp1upd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1fkwcdf</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>Saw inspired nails</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7foy02pq8upd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1fkxm6l</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>Russian Manicure— Update</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fkxm6l</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1fkxm26</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>Russian Manicure— Update</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fkxm26</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1fkxi16</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>Black Stiletto Nails, what do you think?</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qz7zg1wmhupd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1fkx9f0</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>Spooky September Nails</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fkx9f0</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1fkwy7i</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>Latest nails</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/24fyz80rdupd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1fkwq7h</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails for a wedding. </t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fkwq7h</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1fkwkxf</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>Painted my nails 🤩</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yty204jlaupd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1fkwfxo</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Beach nails </t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jo9q9h7h9upd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1fkwa2c</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>Red tips</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fkwa2c</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1fkw9p4</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>Looking for natural looking short nail ideas! 💅🏻💍</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fkw9p4/looking_for_natural_looking_short_nail_ideas/</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1fkw68x</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>Asked for white french tips.... $60 plus tip ....</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fkw68x</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1fkvpy9</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>My beautiful new nails 🎀</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ii9j4bps3upd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1fkvh9q</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Chrome almond French nails 💅 </t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6kaqldjx1upd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1fku6vz</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>There’s something off about the shape, right?</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jgrawrccstpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1fku6r6</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>First fall nails of the season 👻</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ab07epfbstpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1fku3ni</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>Not the best</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kyn921qnrtpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1fktvek</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>These pink stiletto press-ons are my new favorites! But how did I do? Is it a good job, or a sloppy one? Opinions, please!</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fktvek</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1fktrwx</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Glitter and Pearls ✨️ </t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fktrwx</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1fktlyo</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>My first time getting my nails professionally done!! And they’re my natural nails. 🥰🥰</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fktlyo</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1fktigm</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>My shortie torties</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fktigm</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1fkt2zr</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>Fall leaves</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://i.imgur.com/W5VmPNc.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1fksq2o</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>I need advice from fellow nail babes</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fksq2o/i_need_advice_from_fellow_nail_babes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1fkskfu</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>💞 DIY Gel-Ex Set 💞</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fkskfu</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1fkshk2</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>Did my nails myself!</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fkshk2</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1fkshfl</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>First time doing gel x and it was trickier than I thought</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fkshfl</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1fks7qr</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>Are cheap coloured gel polishes good for nail art?</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fks7qr/are_cheap_coloured_gel_polishes_good_for_nail_art/</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1fkryhs</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Wihte </t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cmznqz797tpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1fkrep1</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>My nails tech rocked these!!</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fkrep1</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1fkr9um</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>Went with a nude chrome look</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rdm0a8s32tpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1fkr0mr</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>Rainbow nails with rainbow cat eye, selfmade press ons! So far my favourite</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fkr0mr</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1fkqyhu</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>First time I did a manicure! I'm so in love!!!</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lxvm6u1rzspd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1fkqm2x</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t xml:space="preserve">nail color </t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fkqm2x</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1fkqg11</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>Struggling with using UV Cured Gels</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fkqg11</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1fkq71y</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>🐌🍄</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x6mjvtf8uspd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1fkp91x</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Twilight set I did! Swipe to see a surprise </t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fkp91x</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1fkp599</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>Can you us base gel under press-ons?</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fkp599/can_you_us_base_gel_under_pressons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1fkpv6n</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>Are they as bad as I think they are 😒</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fkpv6n</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1fkpmma</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>Can I use UV light for Press on gel nails? (Not the glue, clear coat over nail)</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fkpmma/can_i_use_uv_light_for_press_on_gel_nails_not_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1fkpizj</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>Olive and June press on sticky tabs for nails meant to be glued?</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fkpizj/olive_and_june_press_on_sticky_tabs_for_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1fkot4q</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>Help with nail polish staining &amp; good polish/brands that strengthen nails</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fkot4q</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1fkossg</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>Different types of fake nails</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fkossg/different_types_of_fake_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1fkk9am</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>Hand painted nail art inspired by forest fires</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gsvlfmppkrpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1fkgruw</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>Okay.. Nail Dip Kits, what are we thinking?</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fkgruw/okay_nail_dip_kits_what_are_we_thinking/</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1fkema8</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail bed damage and allergy double whammy </t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fkema8/nail_bed_damage_and_allergy_double_whammy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1fkohkm</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>New set!</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fkohkm</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1fko9h4</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>Thoughts(natural nails)?</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pgdy3m2zfspd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1fknpr2</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I'm obsessed </t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fknpr2</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1fkglgo</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>I need help! I have a builder gel that can only be drilled off, but when i did i drilled my nail plate too and they are sore now. I wanted to do different nails but i can’t now. Please help, does anyone know any products or something else.</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zvghy1x3hqpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1fkhr1d</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>Powder dip nail question</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fkhr1d/powder_dip_nail_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1fkhwv0</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>Do I need to apply base coat over builder gel to paint color gel?</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fkhwv0/do_i_need_to_apply_base_coat_over_builder_gel_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1fkhx7w</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>Hollyhock Leaves are a great fall topper</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fkhx7w</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1fknh3i</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>fall nails🍂❤️</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vpmlvywz9spd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1fkk8kx</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I painted Lydia! Still working on my beetlejuice set only one more to go! (These are NOT meant for daily wear y'all it's art/fun) </t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/f9jxunzlkrpd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1fkkt89</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail growth progress </t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2vuwofyeprpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1fkn8eh</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>My latest acrylic nail set done by me</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mk2vu0q68spd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1fl6wzo</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>Nail polish equivalent of MAC lipstick in shade "Mull It To The Max" that I can buy in the UK?</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fl6wzo/nail_polish_equivalent_of_mac_lipstick_in_shade/</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1fl6nop</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>💐</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wh06rrc16xpd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1fl6asr</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>Zoya sale</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hckqyc631xpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1fl5i5x</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>waterlilies (an attempt)</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fl5i5x</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1fl3k2v</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>DIY mani, 2nd attempt</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fl1h36</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1fl2kzn</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>{PR} Sassy Sauce | Wicked Sorcery</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fl2kzn</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1fl20qh</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>It’s Showtime!! 🐛🎃</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fl20qh</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1fl1pxb</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>💜💚 Beetlejuice 2 Duo, Painted Polish and Rogue Lacquer collab</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fl1pxb</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1fl0rcj</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>Cuticula mic drop or KBShimmer fillin' groovy?</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fl0rcj/cuticula_mic_drop_or_kbshimmer_fillin_groovy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1fl03vp</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>What types of nail polish are there?</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fl03vp/what_types_of_nail_polish_are_there/</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1fkzgzl</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>This is such a pretty denim color, which I looove for fall!</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c6bvqn4szupd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1fkz897</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>Does anyone know of a good silver chrome nail polish?</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fkz897/does_anyone_know_of_a_good_silver_chrome_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1fkz7co</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>Polished for days</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fkz7co/polished_for_days/</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1fkz6vv</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I am terrible at magnetics still, but here's Clionadh Cosmetics's Psilocybin as requested! </t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fkz6vv</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1fkymjx</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>Tortoise Shell with DIY Jellies</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fkymjx</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1fkyd3h</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>Embracing the Fall shorties!</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/48foxclopupd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1fkxydz</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>pls help w splotchy gel!</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fkxydz</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1fkx457</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>Year of the Dragon</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mw7bz7t3fupd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1fkw7rb</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>🌅🤎 in summer’s heat i learned to dread the comin’ of the night  🤎🌅</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fkw7rb</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1fkw635</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>colors that match the dark red, light red, and yellow in the red dead redemption 2 poster?</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uxn8tb9b7upd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1fkumvi</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cirque — Siren </t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fkumvi</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1fkuj3g</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New favorite metallic: ILNP Heirloom </t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/v4v5w8brutpd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1fkufgs</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>Had my very first job interview today, so I wore my favorite red polish!</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fkufgs</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1fkueb6</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>Flower Child over Psilocybin because I’m feeling psycho-dellic</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/y2y786utttpd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1fku0b6</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>How’d she do?</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fku0b6</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1fktpws</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First Jelly Polish </t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e532cyhzotpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1fkto25</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>☕️Espresso☕️</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fkto25</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1fktj54</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Feeling fall (in my head, it's still summer here) </t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fktj54</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1fksy9u</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>Essie gel couture top coat drying matte?</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fksy9u</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1fksg2m</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>Fall color~!</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n7shqikzatpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1fksd9g</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>ILNP Amber for fall vibes 🎃</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hjcccigeatpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1fksbnm</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>Dark green &amp; holo</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fksbnm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1fks35v</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>Metallic Mega Mix Collection</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fks35v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1fkrjm8</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>Ruined my nail.. How can I fix this?</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fmtdqeo44tpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1fkr3jd</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>Went to a nail salon and was so indecisive they chose the design for me.</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sd5v7bvr0tpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1fkqsvt</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>DIY’d press-ons with soft gel tips and hard gel</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fkqsvt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1fkqfcu</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Goddess of Fire 🔥 </t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fkqfcu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1fkpvdf</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>So dark. So sparkly. I love.</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/w7rnqouwrspd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1fko367</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>Is dark bordeaux appropriate for ...</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fko367/is_dark_bordeaux_appropriate_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1fkns57</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Felt like doing some comparison swatches of ILNP’s four Mega polishes in different lighting. </t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fkns57</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1fknpy1</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>bkl - earth sunderer</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fknpy1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1fkng37</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>Fall Nail glory!</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fxkvjo0s9spd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1fkncs6</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>TIL: French tips are hard!</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fkncs6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1fkn91h</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>Reign + Sour Apple Rings</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/livwcj0b8spd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1fkmekr</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>FINALLY GOT IT!!!</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fkmekr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1fkmb3s</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>ILNP Birthday Suit on ultra short squares</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fkmb3s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1fkm1w4</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>Switching from gel to polish</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fkm1w4/switching_from_gel_to_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1fkly2u</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>Used my old cloth face masks to protect my polish while traveling.</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ttnagd2ayrpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1fklmwm</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>Got soft gel chrome over blue ombré for 250SAR(66USD)</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a0r2jcwvvrpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1fkk8gl</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Finished painting Lydia for a beetlejuice nail set! 😆💕 These nails are not for daily wear y'all just some fun for my page </t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ra322fflkrpd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1fkjooh</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Layering success! </t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aqf5zx6sfrpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1fkj6nb</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>Are there any top coats that won’t cause a linear holographic polish to scatter and look duller, or is this just caused by any coat that will “smooth” the texture? (Orly rubber base + ILNP Evermore + Sally Hansen Insta-Dri)</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fkj6nb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1fkiisy</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>Color question</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fkiisy/color_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1fkhdut</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>Ready for fall 🍁🍂</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fkhdut</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1fkh7ch</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>rhinestones with regular polish</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fkh7ch/rhinestones_with_regular_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1fkh56f</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I got bored and chopped my long nails off </t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fkh56f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1fl6p47</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t xml:space="preserve">keeping it classy 💅 </t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7tl4c5ul6xpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1fl3m07</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t xml:space="preserve">They’re a bit old but… cute? </t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fl3m07</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1fl1ny0</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>did my nails :3</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s2n0ldzbkvpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1fkzwju</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>Latest BeetleJuice nails!</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pw1444un3vpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1fkzaaa</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>My work today, it took me 4 hours but they are worth it. Like? What would they change? 💕🔥</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fkzaaa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1fky7jq</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Glass nails </t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lgbaly5ioupd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1fky78r</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>ICP nails i did today!!!</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/w1c5wtueoupd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1fkva4a</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>I wanted to embody a creepy reptilian.</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8uhpol5f0upd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1fktl1l</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>Band nails</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fktl1l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1fktj3x</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>Stone Roses</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fktj3x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1fktixn</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>Stone Roses</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fktixn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1fktilg</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>Stone Roses</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fktilg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1fkrsdt</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>My nail tech @nails_emmywynn is truly an artist 🎨 Here is my first Halloween set!!</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fkrsdt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1fkr0be</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>It took me 5 hours… but I impressed myself!</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mnmeks940tpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1fkqdds</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Halloween nails. </t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1gocjyzevspd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1fknflo</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>Newbie</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fknflo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1fkn8vs</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>I told her to raise her prices the first time she did my nails 💜</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d32yi35a8spd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1fkmmve</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First fall set 🧡 </t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fkmmve</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1fkmgoz</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>Squishmallow nails I made for a friend!</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pp8dfkda2spd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1fkik1s</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>Trying out french tips at home ♥</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sq0ecz9x4rpd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1fkies7</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Think I'm going mad 😆 </t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fkies7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1fkh6gy</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>Brat summer ain’t over yet!!!</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mzgwmrzzoqpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1fjwvq4</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>My love - Extreme Nails Stockholm</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1fjwvq4/my_love_extreme_nails_stockholm/</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Sep 21 08:08:57 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_09_22.xlsx
+++ b/data/collected_data/2024_09_22.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1046"/>
+  <dimension ref="A1:C1239"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18215,6 +18215,3287 @@
         </is>
       </c>
     </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1flxkhw</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>Shark nails! 🦈✨💕</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/109rbyb774qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1flxd1d</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>A gift from my boyfriend but now I can't do anything with my hands</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/97fr3yhf44qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1flxcxk</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>Glitterrized</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1flxcxk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1flwzun</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New nails in a few hours I'm thinking red! What about you? </t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xdboraqoz3qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1flvpsn</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>Wear Nails Simple White * And * Nail Art Pieces Cross-* Nail Finished Nail Pieces</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/alu8lpcij3qd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1flv2m2</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>Most Fashionable Nail Designs &amp; Ideas for Summer</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ls03v63xb3qd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1fluysp</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>Unexpected French Manicure And French Tip Nail Designs To, 41% OFF</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bkkrm8coa3qd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1fluwb0</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>Fabulous Fall Coffin Nails Designs</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s3iend5m93qd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1flufml</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>Acrylic nails for the first time</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1flufml/acrylic_nails_for_the_first_time/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1fluq9r</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>Best Burgundy Nails</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xocxsqmt73qd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1fluesk</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>Cute Spring Nails Design</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ut1b6keq43qd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1fludex</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>My nail tech is AMAZING (Naturally Nails in Clayton, BC)</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dymw1tod43qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1flucu1</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>my fall nails!!</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1flucu1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1flucm0</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>Press ons?</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oxiyn0ub43qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1flu9cg</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>This is why I don't tend to buy dollar tree polishes. At least the bottles are cute! (And no, they're NOT color changing!)</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1flu9cg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1flu779</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>Nails by me</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1flu779</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1flr6s4</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>where can i find product to make this effect?</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1hxpu7n582qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1fltmn8</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>Do these acrylics make my nails look bulbous or am I overthinking it?</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fltmn8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1fltm9h</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Basic funny bunny </t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lay5xejnw2qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1fltcmt</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Claire’s press ons!!! 🕷️ </t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c9j2px5xt2qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1fltays</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>Shoot for the stars Kirby!</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fltays</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1flt0xe</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Press on nails with builder gel </t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1flt0xe/press_on_nails_with_builder_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1flt0ho</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>Saw vids of people pushing each other and hiding hello kitty Halloween stuff so I’m debuting my hello kitty Halloween set a month in advance. Would love feedback!</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1flt0ho</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1flsuss</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>Hard gel vs acrylic…?</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1flsuss/hard_gel_vs_acrylic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1fls0up</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>I asked for "green and gold" and got...</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h6dmvm3gg2qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1flrpkw</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>Pink Chrome 💕</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iuaypprbd2qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1flq8q1</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Etsy nails continue to enrich my life and save my wallet </t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jwf34e6gz1qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1flqhgd</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>Rant</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1flqhgd/rant/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1flpw25</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>Best glue that saves press ons!</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1flpw25/best_glue_that_saves_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1flppas</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What color goes with this dress? </t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b2v0ck0nu1qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1flplre</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>My first colorful set ✨</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1flplre</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1flpldi</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>The flower glows in the dark!</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1flpldi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1flo5ms</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>Is this terrible or am I overreacting?</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1flo5ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1flpan3</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>Recent designs</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1flpan3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1flp72t</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>pink + silver</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xoajsvi2q1qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1flp3us</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Russian manicure and hard gel I’ll never go back </t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yyg24fo9p1qd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1flourl</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>Do I have to go back..</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1flourl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1flotl7</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>Short vampy look</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1flotl7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1florsg</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>Why is this happening?</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1florsg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1flon43</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>Spring is coming 🦋🌸</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://www.redgifs.com/watch/dismalslipperylangur</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1flobsd</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>What do you think about the nails I did?</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5v3c01ggi1qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1flo9sv</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>Halloween Monster/Zombie/Werewolf/Witch/Vampire Costume Nails</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ibzecbwuh1qd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1flnt5d</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>First time using press on nails, do they look ok?</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1flnt5d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1flno0d</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>I feel like these are really weird</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1flno0d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1flnd5x</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Whyyy do they do this!!! </t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w0j806hja1qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1flnafl</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>Dipped Nail Repair- do you tip?</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1flnafl/dipped_nail_repair_do_you_tip/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1fln88h</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>Made press-ons for SchoolboyQ Blue Lips tour 💙</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fln88h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1flmtux</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>Choconails</t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1flmtux</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1fllu20</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>Ready for Fall</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fllu20</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1fll75e</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>Halloween nail inspo</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fll75e/halloween_nail_inspo/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1flmoud</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Birthday nails! </t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ffjn08c151qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1flm9ad</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>Details...</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/usnz6umm11qd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1flm5cl</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>Fall nails even though it's still 90°</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qrx3ltkr01qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1flm3zq</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>Ocean Nails</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1flm3zq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1fll5hj</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>Suggestion on shape and color?</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fll5hj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1flkydt</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t xml:space="preserve">White chrome </t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fhlfs5qhr0qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1flkxig</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>Hmmmm</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1flkxig/hmmmm/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1flkvzb</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Halloween came early! </t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ppzibnnyq0qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1flkju8</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Billy y Mandy nails </t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1flkju8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1fljzab</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>Big unicorn energy</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/93kmddawj0qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1flj707</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>I want to do something elegant on my nails, any recommendations please?</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/upm0mdzsd0qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1flixqs</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I would like help to take care of my nails. </t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/njff2k5ub0qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1fliwv2</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>Autumn leaves</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fliwv2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1fliurx</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t xml:space="preserve">i hope you guys don’t mind me showing my favorite nails i did on myself :) </t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fliurx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1flipc8</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Not into this design, can I jazz them up somehow at home? </t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ock4kyqz90qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1flik2v</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is there stickers/stencils to help shape coffin nails better? </t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6qfmq36x80qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1fli78e</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ohora nails - n racer 🏁🏎️ </t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fli78e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1fli5l4</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Couldn’t decide between cheetah or French so i did both </t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fli5l4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1fli22f</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>living in florida will not stop me from getting an autumn color 🍂🖤 (color is DND: 754, winter berry)</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fli22f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1flhu52</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>Where do you guys find your nail decoration/toppers?</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1flhu52/where_do_you_guys_find_your_nail_decorationtoppers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1flhpor</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>30 y.o. Male goth kid here. I like doing the green flames on my index and pinkie cuz those are my horns 🤘Black flame on my middle cuz that’s a spicy finger but trying to think of what to do on ring and thumb. Any ideas?</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i1aey9mk20qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1flhlwc</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>does this red suit my skin tone? not sure 😭</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1flhlwc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1flhage</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>Y’all like this ?</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1flhage</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1flh74v</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>Fall leaves</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vv1djerjyzpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1flh3uz</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Show me your short nails 💅🏼 </t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k51j3z8uxzpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1flgtvw</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SO ready for spooky season! </t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lefm8ddqvzpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1flgqnn</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t xml:space="preserve">These are so cute </t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1flgqnn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1fkstz2</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>new press ons!</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kh32pqf8etpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1fkt56w</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>Bartenders with press on nails… how do you do it?</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fkt56w/bartenders_with_press_on_nails_how_do_you_do_it/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1fl23qs</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help me choose </t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/anzbz51hovpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1fl27el</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>my pearl nails paired with white french tip</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lb3pkq16pvpd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1fl7bqg</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>What do I ask for at the salon?</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fl7bqg/what_do_i_ask_for_at_the_salon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1fle9d3</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>Top coat recommendations</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vxc7mh29czpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1fler9h</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>Advice with first fancy nails</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fler9h/advice_with_first_fancy_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1flfvol</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>First time trying press-ons.... a bit hard to get used to.</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ohkwbtigozpd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1flgh2i</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I've just started doing my nails </t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1flgh2i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1flg2yj</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>Beam me up 🛸</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zfpnxd8zpzpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1flf1ob</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>ILNP - Power Surge</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1flf1ob</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1flf0dj</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>🍋‍🟩🍋🍊✨ Citrus Soda Splash✨</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1flf0dj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1fleh5c</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>good, affordable e file recommendations?</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fleh5c/good_affordable_e_file_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1fleezf</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t xml:space="preserve">8 year old me is screaming </t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/h9rjsftddzpd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1flc8i2</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>Just wanted to share</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1flc8i2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1fldarx</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>My almost Halloween nails</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n7bihxhu4zpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1fld05l</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>Dip nails - normal?</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fld05l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1flcuto</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>my first attempt at a structured gel manicure</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kossoywc1zpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1flclnx</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>Today's style choice</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cpc5fs4dzypd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1flcezg</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>Am I tripping or do these have a scent?!</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8w3f7g1xxypd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1flc814</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>Pastel with sparkles ✨</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/limtssbawypd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1flbt9l</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>first set i’ve ever done on myself!! (feat. crooked pinky)</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1flbt9l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>1flbi2b</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>My first Russian 🥰</t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9vcb0vt9qypd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>1flxmj8</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Licking polish? </t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1flxmj8/licking_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>1flx172</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>looking for a thin QDTC</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1flx172/looking_for_a_thin_qdtc/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1flwagm</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>can anyone identify the brand of this nail polish ?</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1flwagm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1flvzqw</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>Flame blown at night &lt;3</t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/boi37me0n3qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>1flvf9p</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>Cirque Cassiopeia ombre magnetisation</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yhi0oeubg3qd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1flug9q</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>In l💟ve with this shifty glow</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1flug9q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1fltpp8</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Shiftiest multi chromes? </t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fltpp8/shiftiest_multi_chromes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1fltogu</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>Favorite base coat that is NOT a bonding one? My nails are peeling :(</t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fltogu/favorite_base_coat_that_is_not_a_bonding_one_my/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1flt4pg</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>Day 6 of this mani!</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1flt4pg/day_6_of_this_mani/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1flsais</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>KBShimmer haul swatch comparisons (including some of the new fall colors)</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kbqkuh94j2qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1fls5j5</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>I finally figured out how to make my manis last</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fls5j5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1fls553</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I don’t know what this claw pose is but jelly nails! </t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fls553</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1flrzjd</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Night Pollinator </t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1flrzjd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1flroa0</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>ISO: a (non-shifty) red magnetic polish</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n0o3gfxzc2qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1flrnry</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>My Halloween haul</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a8814ovuc2qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1flr8gh</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>Fave drugstore brand nudes</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1flr8gh/fave_drugstore_brand_nudes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1flqqan</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Which Cirque Colours are considered “timeless” “must haves”? Not looking for “trendy”, I’d like colours that will always look classy. </t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1flqqan/which_cirque_colours_are_considered_timeless_must/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1flqmv8</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>Help, what can I do? Kinda scared my nail will break lol</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1flqmv8/help_what_can_i_do_kinda_scared_my_nail_will/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1flqm2l</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Canadians! 🇨🇦 What polishes or nail stuff do you buy when you pop over to the US (in store/online)? </t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1flqm2l/canadians_what_polishes_or_nail_stuff_do_you_buy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1flpv7d</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>Have any of you all seen this before?!</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1flpv7d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1flpo8a</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>I Am Alone. I Am... UTTERLY Alone.</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1flpo8a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1flp96z</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>It's time for my post-summer palette cleanser ⚫⚪🩶</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/obc5alglq1qd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1flp8lm</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BKL Haul…I swear no more till Black Friday </t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ww4z7g8gq1qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1flp2c2</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail polish getting matte near cuticles? </t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rcj19jtwo1qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1flou81</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t>Kintsugi inspired nails</t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1flou81</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1flou2x</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>Kintsugi inspired nails</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1flou2x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1flot12</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The leaves are starting to  change 🍃 🍂 🍁 </t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l383gwonm1qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1floo7c</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>Last gasp of Summer before the Autumnal Equinox on Sunday</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1floo7c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1flokpd</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t>Chocolate nail polish</t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1flokpd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1flocpj</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>I want BLUE VELVET!</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1flocpj/i_want_blue_velvet/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1flo16m</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>Blurple, green and a splash of pink</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/i2wxoz7zf1qd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1fln4vy</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>I’m a sucker for a berry color! Especially this time of year 🍓</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z07y6k2n81qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1flmzcl</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>🍂 but who wants to live forever, babe? 🍂</t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ut3iq2oe71qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1flmxc8</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>Checkerboard obsession 🤍</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/onzlr1ky61qd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1flmwph</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Readily available cheap drugstore matte topcoat </t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1flmwph/readily_available_cheap_drugstore_matte_topcoat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1flm5vq</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>In love with this nude for fall 😍</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1flm5vq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1fllpv3</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Did I get sent a vial of ashes? </t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/299gjwsfx0qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1fllkxp</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t>Anyone else love wearing different colors?</t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zdixiu9cw0qd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1flklrx</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>Arcana Lacquer: Down the Riverwell</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1flklrx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1flkl10</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Midnight Spark ⚡️ </t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1flkl10</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1flkibv</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>Fall themed nail stickers</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ib4lqfa0o0qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1flk6mb</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t xml:space="preserve">beautiful colors </t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uqihcddcl0qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1fljtgj</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>What do you with all that polish?</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fljtgj/what_do_you_with_all_that_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1fljoqh</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>Is this a good nude for my skin tone?</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0e678qhyg0qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1fliwmw</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>French tips attempt #2</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fliupt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>1fli2hl</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>A very happy like-400-different-collections launch day to all who celebrate</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fli2hl/a_very_happy_like400differentcollections_launch/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>1fli08c</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>I heard the call go out for dark shorties</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fli08c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1flhyah</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>Iconic polishes</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1flhyah/iconic_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1flhuzh</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>Witchcult Rosewater Park 💚🌹</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1flhuzh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>1flhnob</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>Super Short Skittle Mani</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1flhnob</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>1flh9a8</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t>Essie jelly gloss wear</t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1flh9a8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>1flh0df</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t>There is never a wrong time for moody glitters ✨</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/41wo22r2xzpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>1flgjyc</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>Wasn't a flakie girl til today</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1flgjyc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>1flfv0s</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>Essie lustrous luxury</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1flfv0s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>1flfd5d</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t>Going to an arcade tonight, so I had to wear this one !</t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1flfd5d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>1flfb74</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>Well the skin around my nails ever go back to normal?</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1flfb74</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>1flf2nh</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t>ILNP - Power Surge</t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1flf2nh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>1flej68</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t>Reflective green glitter 🤤🍃</t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1flej68</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>1fle6xz</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>The Celestial Kingdom</t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fle6xz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>1fle04r</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>Strawberry/milky combo from the summer 🍓☁️</t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p4um77mbazpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>1fldiva</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t>Pumpkin Spice Nails</t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fldiva</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>1fldeyw</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>Storage advice</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fldeyw/storage_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>1flce1a</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>Lights Lacquer Autumn dupes</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1flce1a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>1fla7my</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>Matching the towels 😅</t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/50fxrfnheypd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>1fl9imb</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I have discovered putting chrome over French and instead of white I did pink this time </t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h7sndz5b7ypd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>1fkqslz</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>Manucurist - Sauge</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eaycppajyspd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>1fkvatv</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t>Help! Discoloration under gel top coat?</t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fkvatv/help_discoloration_under_gel_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>1fl9114</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>Last days of summer. Simply the Zest</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fl9114</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>1fl7z7w</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>Essie - Row with the flow (8 days on)</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5eeikpchoxpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>1fl7aq7</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t>Can I show you this gorgeous polish even though I'm a nail biter and very messy painter?</t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h3g7iomzexpd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>1fl73cx</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I have boiled it down to 3 gel polish brands that are supposedly hema free, medium priced and ships to Sweden. Please help me rule 2 out! </t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fl73cx/i_have_boiled_it_down_to_3_gel_polish_brands_that/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>1flxjp7</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t xml:space="preserve">So obsessed with my new punk nails </t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1flxjp7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>1flxeqx</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Glitter purple </t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1flxeqx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>1flux8m</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails I’ve done recently all hand painted no stickers any feedback or positive criticism </t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1flux8m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>1fluu9z</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t>Cute Frenchie set I did in my client</t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/84p8hq3m93qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>1flutkv</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>Mario kart nails I did</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x6e5ckle93qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>1flut39</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Haha cute Labor Day set I did </t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ulrxy63993qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>1flusr4</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t>3d fruit nails press ons</t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ias99f5593qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>1flusd2</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hand painted hello kitty and friends </t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k90y94p093qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>1flurw5</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>I’m doing Nemo fanasty nails</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vi27mqdv83qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>1flt9yb</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t>Shoot for the stars Kirby! Criticism is welcome.</t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1flt9yb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>1flswin</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>Decided to experiment with some nail art tonight.</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1flswin</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>1flpp0n</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Beetle juice and Friday </t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1flpp0n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>1fln9op</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>I made press-ons for SchoolboyQ’s Blue Lips Tour 💙</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fln9op</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>1fln4y1</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>Help</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fln4y1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>1fll7vu</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t>I know it's a little soon but I am so excited!</t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qnnip4eit0qd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>1flkcld</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My Marine Corps nails for my son that's a Lance Corporal. I've been doing this since he has been in service 14 months now and counting. </t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e8xwa11sm0qd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>1flh9l5</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t>Fall leaves</t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1flh9l5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>1fleyva</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t xml:space="preserve">8 year old me is screaming </t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/s3ej3z3khzpd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>1fle6vj</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t>Second day attempting nail art</t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9j5c9a2qbzpd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>1fld2nd</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I need a little consultation! </t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1fld2nd/i_need_a_little_consultation/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>1fla55i</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t>Realised too late i spelled Surprise wrong.... Lol</t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fla55i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>1fl8ppi</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>Gyals! Can nailArt look pretty in short ugly nails like mine🥲?</t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j7u6h581yxpd1.png</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Sep 22 08:08:54 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_09_22.xlsx
+++ b/data/collected_data/2024_09_22.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1239"/>
+  <dimension ref="A1:C1419"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -21496,6 +21496,3066 @@
         </is>
       </c>
     </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>1fmnvoz</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New nails! </t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y9c0hogwebqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>1fmmria</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>Are my nails too short for acrylics? (don’t judge me please i know they are bad 😭)</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fmmria</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>1fmm1j0</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I did a thing </t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fmm1j0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>1fmlshz</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fall amber nails </t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fmlshz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>1fmlliw</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t>Nail wraps coming in clutch again… 💅🎃🦇Are you ready for Halloween?</t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fmlliw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>1fmlcds</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t>any fan of Kitty besides me? Did you like them? 💕❤️🎀</t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fmlcds</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>1fml8up</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>green is the color of this season 💚</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fml8up</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>1fmkmvm</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t>is there a pro tip for doing powder nails with a chrome top coat to not chip? #gel #nails #chrome</t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fmkmvm/is_there_a_pro_tip_for_doing_powder_nails_with_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>1fmkgc1</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t>💜</t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tlxneq759aqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>1fmk7i2</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>Which set should I do next?</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fmk7i2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>1fmk0d9</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>Quick sticker press-ons I made for my right hand</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fmk0d9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>1fmjr58</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t>Tried the chromatic aberation trend!</t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wdk4gqen1aqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>1fmjinc</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cat eye jelly nails by the best nail tech in the world </t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rrfosn89z9qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>1fmj9bw</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t>Beetlejuiceeee…yesss</t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fmj9bw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>1fmhmma</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t>Do you think this would work?</t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fmhmma/do_you_think_this_would_work/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>1fmip0b</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t>Greens and golds💚✨</t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h96s6thqq9qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>1fmiowc</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t>Freestyle and a red panda</t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5a5dom8pq9qd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>1fmiag8</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t>New Set for Fall</t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qfvlmb5mm9qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>1fmhzau</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t>(\_/) Miffy</t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zlged3pdj9qd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>1fmhw4o</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t>Acrylic vs dip</t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fmhw4o/acrylic_vs_dip/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>1fmhnob</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t>Getting Spooky</t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fmhnob</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>1fmhlsx</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t>Baby pink nails! Finally got my nails to be naturally longish!</t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fmhlsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>1fmhjbe</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t>tried to paint these like pencil on paper drawings, how did i do?</t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fmhjbe</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>1fmhapt</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t>Bubble Bath in a bubble bath 🛁</t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m8pygxuic9qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>1fmh91x</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t>I drive over 200 miles to see my nail tech</t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fmh91x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>1fmh8ij</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t>New set for the autumn equinox!</t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/urygy0iwb9qd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>1fmh8bp</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t xml:space="preserve">DIY nails + pizza= Saturday night </t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fmh8bp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>1fmgyyj</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t>Has anyone tried gel strips on gel full-cover tips?</t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fmgyyj/has_anyone_tried_gel_strips_on_gel_fullcover_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>1fmgxfk</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t>Valentine's in September ❤️</t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fmgxfk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>1fmgx4i</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cuticle help !?! </t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fmgx4i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr">
+        <is>
+          <t>1fmazdu</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time doing gel by myself. </t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yzch0sr3t7qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr">
+        <is>
+          <t>1fm97wg</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t>Spooky natural nails!</t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fm97wg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr">
+        <is>
+          <t>1fmbi47</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t>Help inspire my next set?</t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/66pno3tfx7qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="inlineStr">
+        <is>
+          <t>1fmc04h</t>
+        </is>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t>Fall Inspired 🍂🍁🧡</t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fmc04h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="inlineStr">
+        <is>
+          <t>1fmfexv</t>
+        </is>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t>I have Hashimotos syndrome, so this is how fast my nails grow out in 11 days</t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2zb8cc4xu8qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="inlineStr">
+        <is>
+          <t>1fmfkxy</t>
+        </is>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t>How can I improve my Press Ons technique?</t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fmfkxy/how_can_i_improve_my_press_ons_technique/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="inlineStr">
+        <is>
+          <t>1fmgkwu</t>
+        </is>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t>Got tips with acrylic overlay for the first time and I absolutely love them!</t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jirl4sgk59qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="inlineStr">
+        <is>
+          <t>1fmgbex</t>
+        </is>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time DIY tortoise nails </t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6qfrrjo439qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="inlineStr">
+        <is>
+          <t>1fmg1ab</t>
+        </is>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Better shaping ft. my insane collection </t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dvhexg1j09qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="inlineStr">
+        <is>
+          <t>1fmfy2d</t>
+        </is>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t>Lost the cord for my UV lamp that i bought in the 2000's what do you guys recommend?</t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fmfy2d/lost_the_cord_for_my_uv_lamp_that_i_bought_in_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="inlineStr">
+        <is>
+          <t>1fmff0r</t>
+        </is>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t xml:space="preserve">translucent vs opaque gel </t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fmff0r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="inlineStr">
+        <is>
+          <t>1fmf6l8</t>
+        </is>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t xml:space="preserve">accidentally matched my new set with my fave handbag </t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fmf6l8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="inlineStr">
+        <is>
+          <t>1fmf47x</t>
+        </is>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t>Was pretty excited about these press ons</t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h7orars9s8qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="inlineStr">
+        <is>
+          <t>1fmexni</t>
+        </is>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t>my first time using rhinestones and i don’t think i’ll ever stop</t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s9f8abvmq8qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="inlineStr">
+        <is>
+          <t>1fmep68</t>
+        </is>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fall two-tone nails 🍂 </t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9x6576pio8qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="inlineStr">
+        <is>
+          <t>1fmeeot</t>
+        </is>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t>First time getting gel BIAB nails, i noticed a gap between my natural nails and the gel, is this normal? Struggling to clean because of the gap!</t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fmeeot</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="inlineStr">
+        <is>
+          <t>1fme99w</t>
+        </is>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Back on my nonsense </t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fme99w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="inlineStr">
+        <is>
+          <t>1fmduhz</t>
+        </is>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t>My chromes become dull</t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ntu112gyg8qd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="inlineStr">
+        <is>
+          <t>1fmdlch</t>
+        </is>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t>My friend has a wedding tonight and I made a set for her to match her dress. I’m obsessed</t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/to50m3jue8qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="inlineStr">
+        <is>
+          <t>1fmdgvb</t>
+        </is>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My new nails </t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fmdgvb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="inlineStr">
+        <is>
+          <t>1fmd720</t>
+        </is>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t>Help</t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8xx46qffb8qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="inlineStr">
+        <is>
+          <t>1fmcteq</t>
+        </is>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t>Loving this new set :33</t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fmcteq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="inlineStr">
+        <is>
+          <t>1fmcoua</t>
+        </is>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t>The first set of Autumn colours</t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fmcoua</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="inlineStr">
+        <is>
+          <t>1fmcj9j</t>
+        </is>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t>PTO time 💅🏽</t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fmcj9j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="inlineStr">
+        <is>
+          <t>1fmcgdn</t>
+        </is>
+      </c>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t>What type of nail shape should I go for?</t>
+        </is>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fmcgdn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="inlineStr">
+        <is>
+          <t>1fmbyev</t>
+        </is>
+      </c>
+      <c r="B1295" t="inlineStr">
+        <is>
+          <t>My beautiful SpongeBob SquarePants nails - "Patrick Star"</t>
+        </is>
+      </c>
+      <c r="C1295" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fmbyev</t>
+        </is>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="inlineStr">
+        <is>
+          <t>1fmbx3z</t>
+        </is>
+      </c>
+      <c r="B1296" t="inlineStr">
+        <is>
+          <t>New press ons!</t>
+        </is>
+      </c>
+      <c r="C1296" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fmbx3z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="inlineStr">
+        <is>
+          <t>1fmbsgb</t>
+        </is>
+      </c>
+      <c r="B1297" t="inlineStr">
+        <is>
+          <t>My latest nails</t>
+        </is>
+      </c>
+      <c r="C1297" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8g3dpd6sz7qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" t="inlineStr">
+        <is>
+          <t>1fmbbku</t>
+        </is>
+      </c>
+      <c r="B1298" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Autumn browns! </t>
+        </is>
+      </c>
+      <c r="C1298" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tznsv2jvv7qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" t="inlineStr">
+        <is>
+          <t>1fmb1a9</t>
+        </is>
+      </c>
+      <c r="B1299" t="inlineStr">
+        <is>
+          <t>What do you think?</t>
+        </is>
+      </c>
+      <c r="C1299" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ydts4klit7qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" t="inlineStr">
+        <is>
+          <t>1fmaxqy</t>
+        </is>
+      </c>
+      <c r="B1300" t="inlineStr">
+        <is>
+          <t>French 💅🏾💕🫶🏽✨</t>
+        </is>
+      </c>
+      <c r="C1300" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9s86ihjps7qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" t="inlineStr">
+        <is>
+          <t>1fmat6m</t>
+        </is>
+      </c>
+      <c r="B1301" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Haven’t been this happy with my nails all year </t>
+        </is>
+      </c>
+      <c r="C1301" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fmat6m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" t="inlineStr">
+        <is>
+          <t>1fmaso3</t>
+        </is>
+      </c>
+      <c r="B1302" t="inlineStr">
+        <is>
+          <t>Aquarelle for Autumn</t>
+        </is>
+      </c>
+      <c r="C1302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fmaso3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" t="inlineStr">
+        <is>
+          <t>1fmamnx</t>
+        </is>
+      </c>
+      <c r="B1303" t="inlineStr">
+        <is>
+          <t>Spooky season!! New set Glamnetic Harry Potter nails 💅🏼🖤💀🖤</t>
+        </is>
+      </c>
+      <c r="C1303" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rcrbt453q7qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" t="inlineStr">
+        <is>
+          <t>1fmagh1</t>
+        </is>
+      </c>
+      <c r="B1304" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Bday nails </t>
+        </is>
+      </c>
+      <c r="C1304" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uxyimddno7qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" t="inlineStr">
+        <is>
+          <t>1fma9cf</t>
+        </is>
+      </c>
+      <c r="B1305" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Chrome green tips </t>
+        </is>
+      </c>
+      <c r="C1305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fma9cf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" t="inlineStr">
+        <is>
+          <t>1fm9ksw</t>
+        </is>
+      </c>
+      <c r="B1306" t="inlineStr">
+        <is>
+          <t>I sadly can’t do nail art but love a good nude 🥰</t>
+        </is>
+      </c>
+      <c r="C1306" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/am3ahfyfh7qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" t="inlineStr">
+        <is>
+          <t>1fm9hdh</t>
+        </is>
+      </c>
+      <c r="B1307" t="inlineStr">
+        <is>
+          <t>my hummingmint nails‧₊˚ೀ⋆｡</t>
+        </is>
+      </c>
+      <c r="C1307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fm9hdh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" t="inlineStr">
+        <is>
+          <t>1fm98a5</t>
+        </is>
+      </c>
+      <c r="B1308" t="inlineStr">
+        <is>
+          <t>$45 for this Press on Nails, what do you think?</t>
+        </is>
+      </c>
+      <c r="C1308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fm98a5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" t="inlineStr">
+        <is>
+          <t>1fm934s</t>
+        </is>
+      </c>
+      <c r="B1309" t="inlineStr">
+        <is>
+          <t>my first spooky set!!</t>
+        </is>
+      </c>
+      <c r="C1309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fm934s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" t="inlineStr">
+        <is>
+          <t>1fm8kk2</t>
+        </is>
+      </c>
+      <c r="B1310" t="inlineStr">
+        <is>
+          <t>Which shape would be good?</t>
+        </is>
+      </c>
+      <c r="C1310" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vdqtethb97qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" t="inlineStr">
+        <is>
+          <t>1fm8c7g</t>
+        </is>
+      </c>
+      <c r="B1311" t="inlineStr">
+        <is>
+          <t>tortoise shell freestyle🤎🧸☕️</t>
+        </is>
+      </c>
+      <c r="C1311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fm8c7g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" t="inlineStr">
+        <is>
+          <t>1fm89n5</t>
+        </is>
+      </c>
+      <c r="B1312" t="inlineStr">
+        <is>
+          <t>I am obsessed with this shape</t>
+        </is>
+      </c>
+      <c r="C1312" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3efap7zu67qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1313">
+      <c r="A1313" t="inlineStr">
+        <is>
+          <t>1fm7uhf</t>
+        </is>
+      </c>
+      <c r="B1313" t="inlineStr">
+        <is>
+          <t>My nail is lifting and it’s like half off but half not, if my nail hits anything it’s really bad, how can I get off?</t>
+        </is>
+      </c>
+      <c r="C1313" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/um354aeg37qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1314">
+      <c r="A1314" t="inlineStr">
+        <is>
+          <t>1fm7je5</t>
+        </is>
+      </c>
+      <c r="B1314" t="inlineStr">
+        <is>
+          <t>Drug store press ons?</t>
+        </is>
+      </c>
+      <c r="C1314" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fm7je5/drug_store_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1315">
+      <c r="A1315" t="inlineStr">
+        <is>
+          <t>1fm7059</t>
+        </is>
+      </c>
+      <c r="B1315" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I tried to recreate a post from here that I loved. We are slowly getting ready for autumn! </t>
+        </is>
+      </c>
+      <c r="C1315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fm7059</t>
+        </is>
+      </c>
+    </row>
+    <row r="1316">
+      <c r="A1316" t="inlineStr">
+        <is>
+          <t>1fm6vz8</t>
+        </is>
+      </c>
+      <c r="B1316" t="inlineStr">
+        <is>
+          <t>Chrome nails at home</t>
+        </is>
+      </c>
+      <c r="C1316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fm6vz8/chrome_nails_at_home/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1317">
+      <c r="A1317" t="inlineStr">
+        <is>
+          <t>1fm6hdq</t>
+        </is>
+      </c>
+      <c r="B1317" t="inlineStr">
+        <is>
+          <t>Really loving this cosmic/witchy purple sparkle</t>
+        </is>
+      </c>
+      <c r="C1317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fm6hdq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1318">
+      <c r="A1318" t="inlineStr">
+        <is>
+          <t>1fm6exw</t>
+        </is>
+      </c>
+      <c r="B1318" t="inlineStr">
+        <is>
+          <t>Dam Nail Polish - Twinkling Tornado 🌪️</t>
+        </is>
+      </c>
+      <c r="C1318" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fm6exw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1319">
+      <c r="A1319" t="inlineStr">
+        <is>
+          <t>1fm5ldi</t>
+        </is>
+      </c>
+      <c r="B1319" t="inlineStr">
+        <is>
+          <t>my favorite set to date 🧚</t>
+        </is>
+      </c>
+      <c r="C1319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fm5ldi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1320">
+      <c r="A1320" t="inlineStr">
+        <is>
+          <t>1fm59bw</t>
+        </is>
+      </c>
+      <c r="B1320" t="inlineStr">
+        <is>
+          <t>Cheshire Tortie</t>
+        </is>
+      </c>
+      <c r="C1320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fm59bw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1321">
+      <c r="A1321" t="inlineStr">
+        <is>
+          <t>1fm4rj0</t>
+        </is>
+      </c>
+      <c r="B1321" t="inlineStr">
+        <is>
+          <t>Time for fall! 🍂</t>
+        </is>
+      </c>
+      <c r="C1321" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kurh9wuce6qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1322">
+      <c r="A1322" t="inlineStr">
+        <is>
+          <t>1fm4gnr</t>
+        </is>
+      </c>
+      <c r="B1322" t="inlineStr">
+        <is>
+          <t>My birthday nails</t>
+        </is>
+      </c>
+      <c r="C1322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fm4gnr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1323">
+      <c r="A1323" t="inlineStr">
+        <is>
+          <t>1fm4ece</t>
+        </is>
+      </c>
+      <c r="B1323" t="inlineStr">
+        <is>
+          <t>Still practicing with lacquer and not the best pictures but fall is here!</t>
+        </is>
+      </c>
+      <c r="C1323" t="inlineStr">
+        <is>
+          <t>https://www.imgur.com/a/CEOZfti</t>
+        </is>
+      </c>
+    </row>
+    <row r="1324">
+      <c r="A1324" t="inlineStr">
+        <is>
+          <t>1fm4du3</t>
+        </is>
+      </c>
+      <c r="B1324" t="inlineStr">
+        <is>
+          <t>Autumn nails</t>
+        </is>
+      </c>
+      <c r="C1324" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6lo0zv74b6qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1325">
+      <c r="A1325" t="inlineStr">
+        <is>
+          <t>1fm48hh</t>
+        </is>
+      </c>
+      <c r="B1325" t="inlineStr">
+        <is>
+          <t>Catching Dreams in Fall</t>
+        </is>
+      </c>
+      <c r="C1325" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fkst54uu96qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1326">
+      <c r="A1326" t="inlineStr">
+        <is>
+          <t>1fm3ke1</t>
+        </is>
+      </c>
+      <c r="B1326" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Art historical press-ons for the art historian </t>
+        </is>
+      </c>
+      <c r="C1326" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7b0cacu846qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1327">
+      <c r="A1327" t="inlineStr">
+        <is>
+          <t>1fm3jri</t>
+        </is>
+      </c>
+      <c r="B1327" t="inlineStr">
+        <is>
+          <t>Got my first ever acrylics!! Then realized where my nailspo came from 💜</t>
+        </is>
+      </c>
+      <c r="C1327" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fl0oj5ex36qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1328">
+      <c r="A1328" t="inlineStr">
+        <is>
+          <t>1fm2pg2</t>
+        </is>
+      </c>
+      <c r="B1328" t="inlineStr">
+        <is>
+          <t>👻🖤😍</t>
+        </is>
+      </c>
+      <c r="C1328" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eirydlupw5qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1329">
+      <c r="A1329" t="inlineStr">
+        <is>
+          <t>1fm2g65</t>
+        </is>
+      </c>
+      <c r="B1329" t="inlineStr">
+        <is>
+          <t>My 3rd successful set of Impress Nails</t>
+        </is>
+      </c>
+      <c r="C1329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fm2g65</t>
+        </is>
+      </c>
+    </row>
+    <row r="1330">
+      <c r="A1330" t="inlineStr">
+        <is>
+          <t>1fm21f2</t>
+        </is>
+      </c>
+      <c r="B1330" t="inlineStr">
+        <is>
+          <t>Dark moment</t>
+        </is>
+      </c>
+      <c r="C1330" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a6rvymoeq5qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1331">
+      <c r="A1331" t="inlineStr">
+        <is>
+          <t>1fm1vor</t>
+        </is>
+      </c>
+      <c r="B1331" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time doing French Tips, How did I do? </t>
+        </is>
+      </c>
+      <c r="C1331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fm1vor</t>
+        </is>
+      </c>
+    </row>
+    <row r="1332">
+      <c r="A1332" t="inlineStr">
+        <is>
+          <t>1fm1ogn</t>
+        </is>
+      </c>
+      <c r="B1332" t="inlineStr">
+        <is>
+          <t>Update on my first time doing press on nails (I already know that hey still look bad)</t>
+        </is>
+      </c>
+      <c r="C1332" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5m2leaesm5qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1333">
+      <c r="A1333" t="inlineStr">
+        <is>
+          <t>1fm1dgc</t>
+        </is>
+      </c>
+      <c r="B1333" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I GOT RED! </t>
+        </is>
+      </c>
+      <c r="C1333" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3z00ed5nj5qd1.gif</t>
+        </is>
+      </c>
+    </row>
+    <row r="1334">
+      <c r="A1334" t="inlineStr">
+        <is>
+          <t>1fm1bvj</t>
+        </is>
+      </c>
+      <c r="B1334" t="inlineStr">
+        <is>
+          <t>My soft pink nails with a French touch! 🌸</t>
+        </is>
+      </c>
+      <c r="C1334" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/szq6au26j5qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1335">
+      <c r="A1335" t="inlineStr">
+        <is>
+          <t>1fm14du</t>
+        </is>
+      </c>
+      <c r="B1335" t="inlineStr">
+        <is>
+          <t>CAT EYE NAILS! Don’t know how to pose them to show the effect.</t>
+        </is>
+      </c>
+      <c r="C1335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fm14du</t>
+        </is>
+      </c>
+    </row>
+    <row r="1336">
+      <c r="A1336" t="inlineStr">
+        <is>
+          <t>1fm0jr3</t>
+        </is>
+      </c>
+      <c r="B1336" t="inlineStr">
+        <is>
+          <t>Would this pattern work on nails? What is it called?</t>
+        </is>
+      </c>
+      <c r="C1336" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bvh0kjtba5qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1337">
+      <c r="A1337" t="inlineStr">
+        <is>
+          <t>1fm0fy5</t>
+        </is>
+      </c>
+      <c r="B1337" t="inlineStr">
+        <is>
+          <t>What does doing your nails mean to you?</t>
+        </is>
+      </c>
+      <c r="C1337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fm0fy5/what_does_doing_your_nails_mean_to_you/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1338">
+      <c r="A1338" t="inlineStr">
+        <is>
+          <t>1fm0e3e</t>
+        </is>
+      </c>
+      <c r="B1338" t="inlineStr">
+        <is>
+          <t>Fall is officially here</t>
+        </is>
+      </c>
+      <c r="C1338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fm0e3e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1339">
+      <c r="A1339" t="inlineStr">
+        <is>
+          <t>1fm09kr</t>
+        </is>
+      </c>
+      <c r="B1339" t="inlineStr">
+        <is>
+          <t>Pink Chrome Nails</t>
+        </is>
+      </c>
+      <c r="C1339" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fkvwwhov65qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1340">
+      <c r="A1340" t="inlineStr">
+        <is>
+          <t>1fmo6zh</t>
+        </is>
+      </c>
+      <c r="B1340" t="inlineStr">
+        <is>
+          <t>Holo Taco at Ulta?!</t>
+        </is>
+      </c>
+      <c r="C1340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fmo6zh/holo_taco_at_ulta/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1341">
+      <c r="A1341" t="inlineStr">
+        <is>
+          <t>1fmnzv6</t>
+        </is>
+      </c>
+      <c r="B1341" t="inlineStr">
+        <is>
+          <t>Clarins 230: to fix or to topper??</t>
+        </is>
+      </c>
+      <c r="C1341" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vgku8jvggbqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1342">
+      <c r="A1342" t="inlineStr">
+        <is>
+          <t>1fmm3rt</t>
+        </is>
+      </c>
+      <c r="B1342" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What’s the deal with matte polish? </t>
+        </is>
+      </c>
+      <c r="C1342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fmm3rt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1343">
+      <c r="A1343" t="inlineStr">
+        <is>
+          <t>1fmlc62</t>
+        </is>
+      </c>
+      <c r="B1343" t="inlineStr">
+        <is>
+          <t>Divot in fingernail edge no matter what I do???</t>
+        </is>
+      </c>
+      <c r="C1343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fmlc62</t>
+        </is>
+      </c>
+    </row>
+    <row r="1344">
+      <c r="A1344" t="inlineStr">
+        <is>
+          <t>1fmkuxp</t>
+        </is>
+      </c>
+      <c r="B1344" t="inlineStr">
+        <is>
+          <t>Finally got my hands on Goblins and Ghoulies and it was so worth it!</t>
+        </is>
+      </c>
+      <c r="C1344" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/chnyvb9ndaqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1345">
+      <c r="A1345" t="inlineStr">
+        <is>
+          <t>1fmkd2w</t>
+        </is>
+      </c>
+      <c r="B1345" t="inlineStr">
+        <is>
+          <t>Who knew that a cute customer would stop over a decade of nail picking (nail picking to clean and smooth cuticles)</t>
+        </is>
+      </c>
+      <c r="C1345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fmkd2w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1346">
+      <c r="A1346" t="inlineStr">
+        <is>
+          <t>1fmkbir</t>
+        </is>
+      </c>
+      <c r="B1346" t="inlineStr">
+        <is>
+          <t>🌸🏜</t>
+        </is>
+      </c>
+      <c r="C1346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fmkbir</t>
+        </is>
+      </c>
+    </row>
+    <row r="1347">
+      <c r="A1347" t="inlineStr">
+        <is>
+          <t>1fmk71n</t>
+        </is>
+      </c>
+      <c r="B1347" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Top coat recommendations </t>
+        </is>
+      </c>
+      <c r="C1347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fmk71n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1348">
+      <c r="A1348" t="inlineStr">
+        <is>
+          <t>1fmhwu0</t>
+        </is>
+      </c>
+      <c r="B1348" t="inlineStr">
+        <is>
+          <t>A Magenta shade (I think)</t>
+        </is>
+      </c>
+      <c r="C1348" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nsoy5rgni9qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1349">
+      <c r="A1349" t="inlineStr">
+        <is>
+          <t>1fmh46u</t>
+        </is>
+      </c>
+      <c r="B1349" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Am I using my thermal wrong? </t>
+        </is>
+      </c>
+      <c r="C1349" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fmh46u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1350">
+      <c r="A1350" t="inlineStr">
+        <is>
+          <t>1fmgu5p</t>
+        </is>
+      </c>
+      <c r="B1350" t="inlineStr">
+        <is>
+          <t>Sunflower Water Decals over stamped checkerboard</t>
+        </is>
+      </c>
+      <c r="C1350" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qy08vmz089qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1351">
+      <c r="A1351" t="inlineStr">
+        <is>
+          <t>1fmgt9n</t>
+        </is>
+      </c>
+      <c r="B1351" t="inlineStr">
+        <is>
+          <t>A few of my favorite things! (spoiler 2nd photo)</t>
+        </is>
+      </c>
+      <c r="C1351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fmgt9n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1352">
+      <c r="A1352" t="inlineStr">
+        <is>
+          <t>1fmgsgq</t>
+        </is>
+      </c>
+      <c r="B1352" t="inlineStr">
+        <is>
+          <t>how often does mooncat change the rewards options?</t>
+        </is>
+      </c>
+      <c r="C1352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fmgsgq/how_often_does_mooncat_change_the_rewards_options/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1353">
+      <c r="A1353" t="inlineStr">
+        <is>
+          <t>1fmfyoo</t>
+        </is>
+      </c>
+      <c r="B1353" t="inlineStr">
+        <is>
+          <t>Looking for a Purple Disturbia dupe</t>
+        </is>
+      </c>
+      <c r="C1353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fmfyoo/looking_for_a_purple_disturbia_dupe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1354">
+      <c r="A1354" t="inlineStr">
+        <is>
+          <t>1fmfudz</t>
+        </is>
+      </c>
+      <c r="B1354" t="inlineStr">
+        <is>
+          <t>Facebook Marketplace Haul! 💓💓</t>
+        </is>
+      </c>
+      <c r="C1354" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3iuvl00sy8qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1355">
+      <c r="A1355" t="inlineStr">
+        <is>
+          <t>1fmfomw</t>
+        </is>
+      </c>
+      <c r="B1355" t="inlineStr">
+        <is>
+          <t>My first time doing velvet nails! Except for my ring finger which was a failed experiment 😅</t>
+        </is>
+      </c>
+      <c r="C1355" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/oioajppax8qd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1356">
+      <c r="A1356" t="inlineStr">
+        <is>
+          <t>1fmf69x</t>
+        </is>
+      </c>
+      <c r="B1356" t="inlineStr">
+        <is>
+          <t>Your heart is a black hole ♥️</t>
+        </is>
+      </c>
+      <c r="C1356" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fmf69x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1357">
+      <c r="A1357" t="inlineStr">
+        <is>
+          <t>1fmewdq</t>
+        </is>
+      </c>
+      <c r="B1357" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Enjoying the holo magnetic before it fades 😭 </t>
+        </is>
+      </c>
+      <c r="C1357" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/pbkkmcjaq8qd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1358">
+      <c r="A1358" t="inlineStr">
+        <is>
+          <t>1fmer5u</t>
+        </is>
+      </c>
+      <c r="B1358" t="inlineStr">
+        <is>
+          <t>Kozmic Colours Green</t>
+        </is>
+      </c>
+      <c r="C1358" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fmer5u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1359">
+      <c r="A1359" t="inlineStr">
+        <is>
+          <t>1fmenrj</t>
+        </is>
+      </c>
+      <c r="B1359" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Any upcoming sales to be aware of? </t>
+        </is>
+      </c>
+      <c r="C1359" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fmenrj/any_upcoming_sales_to_be_aware_of/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1360">
+      <c r="A1360" t="inlineStr">
+        <is>
+          <t>1fmehkk</t>
+        </is>
+      </c>
+      <c r="B1360" t="inlineStr">
+        <is>
+          <t>Tried using an ombre nail brush</t>
+        </is>
+      </c>
+      <c r="C1360" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6cwb8j9mm8qd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1361">
+      <c r="A1361" t="inlineStr">
+        <is>
+          <t>1fmedce</t>
+        </is>
+      </c>
+      <c r="B1361" t="inlineStr">
+        <is>
+          <t>Holo Texture?</t>
+        </is>
+      </c>
+      <c r="C1361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fmedce/holo_texture/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1362">
+      <c r="A1362" t="inlineStr">
+        <is>
+          <t>1fmdv5d</t>
+        </is>
+      </c>
+      <c r="B1362" t="inlineStr">
+        <is>
+          <t>Please help, my chromes become dull</t>
+        </is>
+      </c>
+      <c r="C1362" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ioppgcg4h8qd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1363">
+      <c r="A1363" t="inlineStr">
+        <is>
+          <t>1fmdqv4</t>
+        </is>
+      </c>
+      <c r="B1363" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pure Falloween </t>
+        </is>
+      </c>
+      <c r="C1363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fmdqv4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1364">
+      <c r="A1364" t="inlineStr">
+        <is>
+          <t>1fmcz53</t>
+        </is>
+      </c>
+      <c r="B1364" t="inlineStr">
+        <is>
+          <t>Orly's Nouveau Riche</t>
+        </is>
+      </c>
+      <c r="C1364" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ngjj7w5k98qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1365">
+      <c r="A1365" t="inlineStr">
+        <is>
+          <t>1fmct5o</t>
+        </is>
+      </c>
+      <c r="B1365" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tried Clionadh's magnetic polish </t>
+        </is>
+      </c>
+      <c r="C1365" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fmct5o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1366">
+      <c r="A1366" t="inlineStr">
+        <is>
+          <t>1fmc92b</t>
+        </is>
+      </c>
+      <c r="B1366" t="inlineStr">
+        <is>
+          <t>Ivy League</t>
+        </is>
+      </c>
+      <c r="C1366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fmc92b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1367">
+      <c r="A1367" t="inlineStr">
+        <is>
+          <t>1fmc3ps</t>
+        </is>
+      </c>
+      <c r="B1367" t="inlineStr">
+        <is>
+          <t>Bugs and Flowers</t>
+        </is>
+      </c>
+      <c r="C1367" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fmc3ps</t>
+        </is>
+      </c>
+    </row>
+    <row r="1368">
+      <c r="A1368" t="inlineStr">
+        <is>
+          <t>1fmbqe4</t>
+        </is>
+      </c>
+      <c r="B1368" t="inlineStr">
+        <is>
+          <t>Cheek/lip stain as nail color?</t>
+        </is>
+      </c>
+      <c r="C1368" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dk6j87c7z7qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1369">
+      <c r="A1369" t="inlineStr">
+        <is>
+          <t>1fmbogr</t>
+        </is>
+      </c>
+      <c r="B1369" t="inlineStr">
+        <is>
+          <t>Anticipating the cooler weather finally coming in this weekend</t>
+        </is>
+      </c>
+      <c r="C1369" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mhpf5qavy7qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1370">
+      <c r="A1370" t="inlineStr">
+        <is>
+          <t>1fmbhs4</t>
+        </is>
+      </c>
+      <c r="B1370" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Recently moved continents and couldn't bring any polish with me. So I splurged a little to celebrate new beginnings </t>
+        </is>
+      </c>
+      <c r="C1370" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0gzo98adx7qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1371">
+      <c r="A1371" t="inlineStr">
+        <is>
+          <t>1fmb9m9</t>
+        </is>
+      </c>
+      <c r="B1371" t="inlineStr">
+        <is>
+          <t>Thinking of June Bugs 🪲 Gingko Leaf &amp; Serpentine Polish</t>
+        </is>
+      </c>
+      <c r="C1371" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fmb9m9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1372">
+      <c r="A1372" t="inlineStr">
+        <is>
+          <t>1fmayzh</t>
+        </is>
+      </c>
+      <c r="B1372" t="inlineStr">
+        <is>
+          <t>Pahlish - Red Wine Supernova</t>
+        </is>
+      </c>
+      <c r="C1372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fmayzh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1373">
+      <c r="A1373" t="inlineStr">
+        <is>
+          <t>1fmas8c</t>
+        </is>
+      </c>
+      <c r="B1373" t="inlineStr">
+        <is>
+          <t>pink skittle 🩷</t>
+        </is>
+      </c>
+      <c r="C1373" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bdrd4fler7qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1374">
+      <c r="A1374" t="inlineStr">
+        <is>
+          <t>1fm9jsf</t>
+        </is>
+      </c>
+      <c r="B1374" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I am doing a series of manis inspired by books - this one is inspired by The Spear Cuts Through Water by Simon Jimenez </t>
+        </is>
+      </c>
+      <c r="C1374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fm9jsf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1375">
+      <c r="A1375" t="inlineStr">
+        <is>
+          <t>1fm9e00</t>
+        </is>
+      </c>
+      <c r="B1375" t="inlineStr">
+        <is>
+          <t>Quick emotional check-in.</t>
+        </is>
+      </c>
+      <c r="C1375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fm9e00/quick_emotional_checkin/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1376">
+      <c r="A1376" t="inlineStr">
+        <is>
+          <t>1fm936m</t>
+        </is>
+      </c>
+      <c r="B1376" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I’m obsessed with shimmer toppers. I want more colors, any suggestions? </t>
+        </is>
+      </c>
+      <c r="C1376" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2sb3rfjhd7qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1377">
+      <c r="A1377" t="inlineStr">
+        <is>
+          <t>1fm8wli</t>
+        </is>
+      </c>
+      <c r="B1377" t="inlineStr">
+        <is>
+          <t>A simple red holo hits the spot today ❤️</t>
+        </is>
+      </c>
+      <c r="C1377" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/53my8ze1c7qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1378">
+      <c r="A1378" t="inlineStr">
+        <is>
+          <t>1fm881k</t>
+        </is>
+      </c>
+      <c r="B1378" t="inlineStr">
+        <is>
+          <t>Looking for dupe suggestions: Ciaté's LA Confidential</t>
+        </is>
+      </c>
+      <c r="C1378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fm881k/looking_for_dupe_suggestions_ciatés_la/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1379">
+      <c r="A1379" t="inlineStr">
+        <is>
+          <t>1fm84cg</t>
+        </is>
+      </c>
+      <c r="B1379" t="inlineStr">
+        <is>
+          <t>I painted my husband's nails last night and today he asked me to order him more colors 😇</t>
+        </is>
+      </c>
+      <c r="C1379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fm84cg/i_painted_my_husbands_nails_last_night_and_today/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1380">
+      <c r="A1380" t="inlineStr">
+        <is>
+          <t>1fm815h</t>
+        </is>
+      </c>
+      <c r="B1380" t="inlineStr">
+        <is>
+          <t>Rogue Lacquer “Squish”</t>
+        </is>
+      </c>
+      <c r="C1380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fm815h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1381">
+      <c r="A1381" t="inlineStr">
+        <is>
+          <t>1fm80v8</t>
+        </is>
+      </c>
+      <c r="B1381" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Haven’t painted my nails in such a long time. But felt like it was finally time to do so. ILNP Poppy. </t>
+        </is>
+      </c>
+      <c r="C1381" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f3swdmow47qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1382">
+      <c r="A1382" t="inlineStr">
+        <is>
+          <t>1fm7ywh</t>
+        </is>
+      </c>
+      <c r="B1382" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My daughter is ONE OF US! Fire 🔥 Water 💧 </t>
+        </is>
+      </c>
+      <c r="C1382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fm7ywh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1383">
+      <c r="A1383" t="inlineStr">
+        <is>
+          <t>1fm7kcl</t>
+        </is>
+      </c>
+      <c r="B1383" t="inlineStr">
+        <is>
+          <t>Saturday Mani Part Two: Access Denied/Good Fortune topped with Maelstrom by Mooncat</t>
+        </is>
+      </c>
+      <c r="C1383" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6zky7ue617qd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1384">
+      <c r="A1384" t="inlineStr">
+        <is>
+          <t>1fm7iby</t>
+        </is>
+      </c>
+      <c r="B1384" t="inlineStr">
+        <is>
+          <t>Saturday Mani Part One: Access Denied by Mooncat mixed with Good Fortune by ILNP</t>
+        </is>
+      </c>
+      <c r="C1384" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/lp3bdxnp07qd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1385">
+      <c r="A1385" t="inlineStr">
+        <is>
+          <t>1fm7ba8</t>
+        </is>
+      </c>
+      <c r="B1385" t="inlineStr">
+        <is>
+          <t>Omg Psilocybin is everything!!</t>
+        </is>
+      </c>
+      <c r="C1385" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0yrxdc98z6qd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1386">
+      <c r="A1386" t="inlineStr">
+        <is>
+          <t>1fm79xr</t>
+        </is>
+      </c>
+      <c r="B1386" t="inlineStr">
+        <is>
+          <t>What causes this?</t>
+        </is>
+      </c>
+      <c r="C1386" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z5ys2s1yy6qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1387">
+      <c r="A1387" t="inlineStr">
+        <is>
+          <t>1fm6vnz</t>
+        </is>
+      </c>
+      <c r="B1387" t="inlineStr">
+        <is>
+          <t>Hot Topic brand is hit-or-miss, but this one sunk my battleship.</t>
+        </is>
+      </c>
+      <c r="C1387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fm6vnz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1388">
+      <c r="A1388" t="inlineStr">
+        <is>
+          <t>1fm6plx</t>
+        </is>
+      </c>
+      <c r="B1388" t="inlineStr">
+        <is>
+          <t>MadamGlam shipping and Canadian Customs</t>
+        </is>
+      </c>
+      <c r="C1388" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fm6plx/madamglam_shipping_and_canadian_customs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1389">
+      <c r="A1389" t="inlineStr">
+        <is>
+          <t>1fm6k41</t>
+        </is>
+      </c>
+      <c r="B1389" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Wanted something moody today </t>
+        </is>
+      </c>
+      <c r="C1389" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6x96uro1t6qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1390">
+      <c r="A1390" t="inlineStr">
+        <is>
+          <t>1fm6gxk</t>
+        </is>
+      </c>
+      <c r="B1390" t="inlineStr">
+        <is>
+          <t>Dam Nail Polish - Twinkling Tornado 🌪️</t>
+        </is>
+      </c>
+      <c r="C1390" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fm6gxk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1391">
+      <c r="A1391" t="inlineStr">
+        <is>
+          <t>1fm6dr0</t>
+        </is>
+      </c>
+      <c r="B1391" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Whoa </t>
+        </is>
+      </c>
+      <c r="C1391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fm6dr0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1392">
+      <c r="A1392" t="inlineStr">
+        <is>
+          <t>1fm65xh</t>
+        </is>
+      </c>
+      <c r="B1392" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Bee’s knees sky fire </t>
+        </is>
+      </c>
+      <c r="C1392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fm65xh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1393">
+      <c r="A1393" t="inlineStr">
+        <is>
+          <t>1fm65sy</t>
+        </is>
+      </c>
+      <c r="B1393" t="inlineStr">
+        <is>
+          <t>redemption arc: rotten bananas becoming bread</t>
+        </is>
+      </c>
+      <c r="C1393" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/39w76sovp6qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1394">
+      <c r="A1394" t="inlineStr">
+        <is>
+          <t>1fm5x90</t>
+        </is>
+      </c>
+      <c r="B1394" t="inlineStr">
+        <is>
+          <t>New Great Lakes Lacquer collection Thursday, September 26th @ 9 PM Eastern</t>
+        </is>
+      </c>
+      <c r="C1394" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fm5x90/new_great_lakes_lacquer_collection_thursday/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1395">
+      <c r="A1395" t="inlineStr">
+        <is>
+          <t>1fm5cws</t>
+        </is>
+      </c>
+      <c r="B1395" t="inlineStr">
+        <is>
+          <t>We're Being Elves</t>
+        </is>
+      </c>
+      <c r="C1395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fm5cws</t>
+        </is>
+      </c>
+    </row>
+    <row r="1396">
+      <c r="A1396" t="inlineStr">
+        <is>
+          <t>1fm5csx</t>
+        </is>
+      </c>
+      <c r="B1396" t="inlineStr">
+        <is>
+          <t>brb losing my mind for shimmers and chromes right now</t>
+        </is>
+      </c>
+      <c r="C1396" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fm5csx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1397">
+      <c r="A1397" t="inlineStr">
+        <is>
+          <t>1fm3tvq</t>
+        </is>
+      </c>
+      <c r="B1397" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Talk to me about Great Lakes lacquer </t>
+        </is>
+      </c>
+      <c r="C1397" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fm3tvq/talk_to_me_about_great_lakes_lacquer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1398">
+      <c r="A1398" t="inlineStr">
+        <is>
+          <t>1fm21pd</t>
+        </is>
+      </c>
+      <c r="B1398" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The glow is too strong for the camera </t>
+        </is>
+      </c>
+      <c r="C1398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fm21pd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1399">
+      <c r="A1399" t="inlineStr">
+        <is>
+          <t>1fm06fr</t>
+        </is>
+      </c>
+      <c r="B1399" t="inlineStr">
+        <is>
+          <t>Navy for autumn</t>
+        </is>
+      </c>
+      <c r="C1399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fm06fr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1400">
+      <c r="A1400" t="inlineStr">
+        <is>
+          <t>1flz1mh</t>
+        </is>
+      </c>
+      <c r="B1400" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What’s everyone wearing for fall ? </t>
+        </is>
+      </c>
+      <c r="C1400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1flz1mh/whats_everyone_wearing_for_fall/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1401">
+      <c r="A1401" t="inlineStr">
+        <is>
+          <t>1flyx3u</t>
+        </is>
+      </c>
+      <c r="B1401" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I filed the top of my nails too much and am so stressed </t>
+        </is>
+      </c>
+      <c r="C1401" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1flyx3u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1402">
+      <c r="A1402" t="inlineStr">
+        <is>
+          <t>1flyl0x</t>
+        </is>
+      </c>
+      <c r="B1402" t="inlineStr">
+        <is>
+          <t>$3.25 manicure - sometimes ya get what you pay for 🤡</t>
+        </is>
+      </c>
+      <c r="C1402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1flyl0x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1403">
+      <c r="A1403" t="inlineStr">
+        <is>
+          <t>1flykmy</t>
+        </is>
+      </c>
+      <c r="B1403" t="inlineStr">
+        <is>
+          <t>OPI Hello Kitty in Europe?</t>
+        </is>
+      </c>
+      <c r="C1403" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1flykmy/opi_hello_kitty_in_europe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1404">
+      <c r="A1404" t="inlineStr">
+        <is>
+          <t>1fmie09</t>
+        </is>
+      </c>
+      <c r="B1404" t="inlineStr">
+        <is>
+          <t>First Halloween set of the season!</t>
+        </is>
+      </c>
+      <c r="C1404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fmie09</t>
+        </is>
+      </c>
+    </row>
+    <row r="1405">
+      <c r="A1405" t="inlineStr">
+        <is>
+          <t>1fmfi1u</t>
+        </is>
+      </c>
+      <c r="B1405" t="inlineStr">
+        <is>
+          <t>My first ever Halloween set</t>
+        </is>
+      </c>
+      <c r="C1405" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1j8o9ncov8qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1406">
+      <c r="A1406" t="inlineStr">
+        <is>
+          <t>1fmdtsu</t>
+        </is>
+      </c>
+      <c r="B1406" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My chromes are dulling after top coat </t>
+        </is>
+      </c>
+      <c r="C1406" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jszj1kkqg8qd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1407">
+      <c r="A1407" t="inlineStr">
+        <is>
+          <t>1fmb883</t>
+        </is>
+      </c>
+      <c r="B1407" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Simple Halloween themed nails </t>
+        </is>
+      </c>
+      <c r="C1407" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yjr3na44v7qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1408">
+      <c r="A1408" t="inlineStr">
+        <is>
+          <t>1fmazun</t>
+        </is>
+      </c>
+      <c r="B1408" t="inlineStr">
+        <is>
+          <t>What do you think?</t>
+        </is>
+      </c>
+      <c r="C1408" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cizxm0i7t7qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1409">
+      <c r="A1409" t="inlineStr">
+        <is>
+          <t>1fmatmp</t>
+        </is>
+      </c>
+      <c r="B1409" t="inlineStr">
+        <is>
+          <t>First set of nails that I did in the style I've been working on. What started it all :).</t>
+        </is>
+      </c>
+      <c r="C1409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fmatmp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1410">
+      <c r="A1410" t="inlineStr">
+        <is>
+          <t>1fmar3y</t>
+        </is>
+      </c>
+      <c r="B1410" t="inlineStr">
+        <is>
+          <t>Aquarelle for Autumn</t>
+        </is>
+      </c>
+      <c r="C1410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fmar3y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1411">
+      <c r="A1411" t="inlineStr">
+        <is>
+          <t>1fm9wcn</t>
+        </is>
+      </c>
+      <c r="B1411" t="inlineStr">
+        <is>
+          <t xml:space="preserve">i’m looking for inspo, who is the craziest most skilled nail tech in your country? i’ll start (culturamanicura) </t>
+        </is>
+      </c>
+      <c r="C1411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fm9wcn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1412">
+      <c r="A1412" t="inlineStr">
+        <is>
+          <t>1fm9suu</t>
+        </is>
+      </c>
+      <c r="B1412" t="inlineStr">
+        <is>
+          <t xml:space="preserve">That was hard and time consuming </t>
+        </is>
+      </c>
+      <c r="C1412" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fm9suu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1413">
+      <c r="A1413" t="inlineStr">
+        <is>
+          <t>1fm7zfo</t>
+        </is>
+      </c>
+      <c r="B1413" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First set of press ons! </t>
+        </is>
+      </c>
+      <c r="C1413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fm7zfo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1414">
+      <c r="A1414" t="inlineStr">
+        <is>
+          <t>1fm6pw0</t>
+        </is>
+      </c>
+      <c r="B1414" t="inlineStr">
+        <is>
+          <t>Dream catching Fall</t>
+        </is>
+      </c>
+      <c r="C1414" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/od9vmi9du6qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1415">
+      <c r="A1415" t="inlineStr">
+        <is>
+          <t>1fm6ogg</t>
+        </is>
+      </c>
+      <c r="B1415" t="inlineStr">
+        <is>
+          <t>It’s giving Judy Jetson</t>
+        </is>
+      </c>
+      <c r="C1415" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wput30z1u6qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1416">
+      <c r="A1416" t="inlineStr">
+        <is>
+          <t>1fm6amu</t>
+        </is>
+      </c>
+      <c r="B1416" t="inlineStr">
+        <is>
+          <t>Spooky press ons 👻</t>
+        </is>
+      </c>
+      <c r="C1416" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t5dcepsxq6qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1417">
+      <c r="A1417" t="inlineStr">
+        <is>
+          <t>1fm4igx</t>
+        </is>
+      </c>
+      <c r="B1417" t="inlineStr">
+        <is>
+          <t>Couldn't decide on one cat eye so I did them all!</t>
+        </is>
+      </c>
+      <c r="C1417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fm4igx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1418">
+      <c r="A1418" t="inlineStr">
+        <is>
+          <t>1fm37xh</t>
+        </is>
+      </c>
+      <c r="B1418" t="inlineStr">
+        <is>
+          <t>I made a tutorial of my recent Chappell Roan sword nails and I thought y’all would like to see my process!💖</t>
+        </is>
+      </c>
+      <c r="C1418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fm37xh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1419">
+      <c r="A1419" t="inlineStr">
+        <is>
+          <t>1flym7t</t>
+        </is>
+      </c>
+      <c r="B1419" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail art </t>
+        </is>
+      </c>
+      <c r="C1419" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bkkln259l4qd1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>